<commit_message>
changes for Shabds by occasion
</commit_message>
<xml_diff>
--- a/Video_Poetry.xlsx
+++ b/Video_Poetry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiki/Documents/Personal/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C907E024-2650-CC49-AC1C-2B25E8D45E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F9B1D9-35A0-7344-AEC4-6A17F2221C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22120" activeTab="2" xr2:uid="{8D838E60-7835-F44B-BD1C-2E58B2E8E6E1}"/>
   </bookViews>
@@ -7391,8 +7391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509C33A8-3102-F94A-82D6-D97CE7B00496}">
   <dimension ref="A1:P91"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="K1" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7465,7 +7465,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7519,7 +7519,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bar Bar Kar Jod Kar.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7573,7 +7573,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bhav Bhakti Se Binjan Karti.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>64</v>
       </c>
@@ -7627,7 +7627,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aao Mere Satguru He Meri Jan.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>74</v>
       </c>
@@ -7681,7 +7681,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bar Bar Karoon Binti.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>82</v>
       </c>
@@ -7735,7 +7735,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Mere Anand Anand Bhari.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>260</v>
       </c>
@@ -7789,7 +7789,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Param Purush Pooran Dhani.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>326</v>
       </c>
@@ -7843,7 +7843,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Radhasoami Charan Shish Main Dara.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>477</v>
       </c>
@@ -7897,7 +7897,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Chalo Bidesan Apne Desh.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>478</v>
       </c>
@@ -7951,7 +7951,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Chalo Piyari Apne Ghar.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>483</v>
       </c>
@@ -8005,7 +8005,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Pakado Guru Ke Charan Samhar.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>510</v>
       </c>
@@ -8059,7 +8059,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Khele Surat Guru Charnan Pas.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>547</v>
       </c>
@@ -8113,7 +8113,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Nij Ghar Apne Chal Ri Meri Pyari Suratiya.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>577</v>
       </c>
@@ -8167,7 +8167,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Ghir Aaye Badal Kare.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>578</v>
       </c>
@@ -8221,7 +8221,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Barsat Rimjhim Megha Kare.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>637</v>
       </c>
@@ -8275,7 +8275,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Chhabile Chhavi Lage Tori Pyari.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>638</v>
       </c>
@@ -8329,7 +8329,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Rangile Rang Deo Chunar Hamari.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>652</v>
       </c>
@@ -8383,7 +8383,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Daya Guru Kya Karoon Varnan.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>681</v>
       </c>
@@ -8437,7 +8437,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ke Darshan Karat Rahoon.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>722</v>
       </c>
@@ -8491,7 +8491,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ke Sang Pyari Khelo Phaag.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>738</v>
       </c>
@@ -8545,7 +8545,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ki Mauj Raho Tum Dhar.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>749</v>
       </c>
@@ -8599,7 +8599,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ka Rang Chatakila Kabhi Utre Nahin.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>750</v>
       </c>
@@ -8653,7 +8653,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ka Rang Ati Nirmal.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>841</v>
       </c>
@@ -8707,7 +8707,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Mere Hiye Mein Bajat Badhaee Sant Sang Paya Re.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>845</v>
       </c>
@@ -8761,7 +8761,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Kas Preetam Se Jay Miloon Main.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>865</v>
       </c>
@@ -8815,7 +8815,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jab Se Main Dekha Radhasoami Ka Mukhada.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>916</v>
       </c>
@@ -8869,7 +8869,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Chal Kheliye Satguru Se Rang Holi Aaj Sakhi Ri.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>921</v>
       </c>
@@ -8923,7 +8923,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Tum Socho Apne Man Mein Ya Jag Mein Dukkh Ghanera.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>947</v>
       </c>
@@ -8977,7 +8977,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Aayee Bahar Basant.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>970</v>
       </c>
@@ -9031,7 +9031,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Sang Satguru Kheloongi Hori.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>981</v>
       </c>
@@ -9085,7 +9085,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Aaya Basant Naveen.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>986</v>
       </c>
@@ -9139,7 +9139,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Tadapat Rahi Behal Daras Bin Man Nahin Mane.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1024</v>
       </c>
@@ -9193,7 +9193,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Anand Raha Mauj Se Chahun Dis Chhaee.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1025</v>
       </c>
@@ -9247,7 +9247,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Hangamaye Shadi Ka Garam Ho Raha Dekho Har Ja.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1026</v>
       </c>
@@ -9301,7 +9301,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Guru Pyare Ke Charnon Mein Jhalakati Hai.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1031</v>
       </c>
@@ -9355,7 +9355,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jud Mil Ke Hans Sare Darshan Ko Guru Ke Aaye.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1033</v>
       </c>
@@ -9409,7 +9409,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Yeh Satsang Aur Radhasoami Hai Naam.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1038</v>
       </c>
@@ -9463,7 +9463,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aho Mere Satguru Aho Meri Jan.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1039</v>
       </c>
@@ -9517,7 +9517,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jab Dekha Tej Maine Jo Malik Ke Naam Ka.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1046</v>
       </c>
@@ -9571,7 +9571,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bada Julm Hai Mere Yar.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1054</v>
       </c>
@@ -9625,7 +9625,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Kyon Soch Kare Man Moorakh.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1064</v>
       </c>
@@ -9679,7 +9679,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Achraj Aarat Guru Ki Dharoon.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1078</v>
       </c>
@@ -9733,7 +9733,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bhago Re Jag Se Ab Bhago.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1079</v>
       </c>
@@ -9787,7 +9787,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Cheto Re Ghar Ghat Samharo.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1080</v>
       </c>
@@ -9841,7 +9841,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jago Re Yehan Kab Lag Sona.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1108</v>
       </c>
@@ -9895,7 +9895,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Prem Dat Guru Dijiye Mere Samrath Data Ho.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1128</v>
       </c>
@@ -9949,7 +9949,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/He Mere Samarath Saeen Nij Roop Dikhao.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1130</v>
       </c>
@@ -10003,7 +10003,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jo Mere Preetam Se Preet Kare.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1132</v>
       </c>
@@ -10057,7 +10057,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jagat Jeev Sab Holi Poojen.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1263</v>
       </c>
@@ -10111,7 +10111,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Radhasoami Naam Jo Gave So Hi Tare.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1264</v>
       </c>
@@ -10165,7 +10165,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/NULLVIDEO'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1265</v>
       </c>
@@ -10219,7 +10219,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Badhawa Radhasoami Gaoon.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1266</v>
       </c>
@@ -10273,7 +10273,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Mere Dhoom Bhai Hai Bhari.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1280</v>
       </c>
@@ -10327,7 +10327,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Saj Kar Aarat Laee.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1282</v>
       </c>
@@ -10381,7 +10381,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Anand Mangal Aaj Saj Sab Aarat Laee.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1283</v>
       </c>
@@ -10435,7 +10435,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Karoon Arti Radhasoami Tan Man Surat Lagay.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1291</v>
       </c>
@@ -10489,7 +10489,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aarat Karoon Aaj Satguru Ki.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1301</v>
       </c>
@@ -10543,7 +10543,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Karoon Binti Dou Kar Jori.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1302</v>
       </c>
@@ -10594,7 +10594,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/NULLVIDEO'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1308</v>
       </c>
@@ -10648,7 +10648,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Mere Anand Hot Apar.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1382</v>
       </c>
@@ -10702,7 +10702,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Ki Kar Har Dam Pooja.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1383</v>
       </c>
@@ -10756,7 +10756,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/NULLVIDEO'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1475</v>
       </c>
@@ -10810,7 +10810,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Dard Dukhi Main Birahin Bhari.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1477</v>
       </c>
@@ -10864,7 +10864,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Piya Bin Kaise Jioon Main Pyari.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1479</v>
       </c>
@@ -10918,7 +10918,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Chunar Meri Maili Bhayee.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1484</v>
       </c>
@@ -10972,7 +10972,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Ghadi Ati Pawan Bhavan.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>1485</v>
       </c>
@@ -11026,7 +11026,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Charan Girah Mere Aaye.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>1486</v>
       </c>
@@ -11080,7 +11080,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Kaun Kare Aarat Satguru Ki.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1489</v>
       </c>
@@ -11134,7 +11134,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Main Gunahagar Ati Bhari.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1490</v>
       </c>
@@ -11182,7 +11182,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/NULLVIDEO'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1491</v>
       </c>
@@ -11233,7 +11233,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aarat Gaoon Poore Guru Ki.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1492</v>
       </c>
@@ -11284,7 +11284,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Radhasoami Radhasoami Radhasoami Gaoon.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1494</v>
       </c>
@@ -11335,7 +11335,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Gaoon Arti Lekar Thali.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1507</v>
       </c>
@@ -11386,7 +11386,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Arti Karoon Suhawan.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1529</v>
       </c>
@@ -11440,7 +11440,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ab Man Aatur Daras Pukare.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1530</v>
       </c>
@@ -11491,7 +11491,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ab Main Kaun Kumati Urjhani.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1531</v>
       </c>
@@ -11545,7 +11545,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Karat Hoon Pukar Aaj Suniye Guhar.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1532</v>
       </c>
@@ -11593,7 +11593,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/NULLVIDEO'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1548</v>
       </c>
@@ -11647,7 +11647,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Lagao Meri Naiya Satguru Par.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1553</v>
       </c>
@@ -11701,7 +11701,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Dhiraj Dharana Mat Ghabrana.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1554</v>
       </c>
@@ -11755,7 +11755,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/NULLVIDEO'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1555</v>
       </c>
@@ -11809,7 +11809,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Kaj Mere Kinhe Poore.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1566</v>
       </c>
@@ -11863,7 +11863,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aao Ri Simat He Sakhiyo.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1668</v>
       </c>
@@ -11917,7 +11917,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ghat Mein Kheloon Ab Basant.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1670</v>
       </c>
@@ -11971,7 +11971,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Dekhan Chali Basant Agam Ghar.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1671</v>
       </c>
@@ -12025,7 +12025,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ab Khelat Radhasoami Sang Hori.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1678</v>
       </c>
@@ -12079,7 +12079,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aao Ri Sakhi Jud Holi Gaven.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1683</v>
       </c>
@@ -12133,7 +12133,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ajab Yeh Bangla Liya Sajay.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1712</v>
       </c>
@@ -12187,7 +12187,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Chauka Bartan Kiya Achambhi.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>1714</v>
       </c>
@@ -12241,7 +12241,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bhog Dhare Radhasoami Aage.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1715</v>
       </c>
@@ -12298,13 +12298,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D960A36-6FC1-8340-9C94-9BD4232780B8}">
   <dimension ref="A1:R91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:R91"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="17" width="10.83203125" style="4"/>
+    <col min="1" max="10" width="10.83203125" style="4"/>
+    <col min="11" max="16" width="39.6640625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="4"/>
     <col min="18" max="18" width="10.83203125" style="5"/>
     <col min="19" max="16384" width="10.83203125" style="4"/>
   </cols>
@@ -17274,7 +17276,7 @@
         <v>636</v>
       </c>
       <c r="K2" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A2, """",", ", """", B2, """",", ", """",C2, """",", ", """",D2, """",", ", """",E2, """",", ", """",F2, """",", ", """",G2, """",", ", """",H2, """",", ", """",I2, """",", ", """",J2, """"," ]")</f>
+        <f t="shared" ref="K2:K33" si="0">_xlfn.CONCAT("[ ", """", A2, """",", ", """", B2, """",", ", """",C2, """",", ", """",D2, """",", ", """",E2, """",", ", """",F2, """",", ", """",G2, """",", ", """",H2, """",", ", """",I2, """",", ", """",J2, """"," ]")</f>
         <v>[ "बार बार कर जोड़ कर", "Bar Bar Kar Jod Kar", "राधास्वामी मत पर प्रवचन", "Discourses on Radhasoami Faith", "", "1", "मंगलाचरण एवं बिनती", "Manglacharan and Prayer", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Bar Bar Kar Jod Kar.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bar Bar Kar Jod Kar.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17304,7 +17306,7 @@
         <v>637</v>
       </c>
       <c r="K3" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A3, """",", ", """", B3, """",", ", """",C3, """",", ", """",D3, """",", ", """",E3, """",", ", """",F3, """",", ", """",G3, """",", ", """",H3, """",", ", """",I3, """",", ", """",J3, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "भाव भक्ति से बिंजन करती", "Bhav Bhakti Se Binjan Karti", "नियमावली", "Sar Bachan Chand Band Part 2", "", "", "भोग, नियमावली", "Bhog, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Bhav Bhakti Se Binjan Karti.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bhav Bhakti Se Binjan Karti.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17340,7 +17342,7 @@
         <v>638</v>
       </c>
       <c r="K4" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A4, """",", ", """", B4, """",", ", """",C4, """",", ", """",D4, """",", ", """",E4, """",", ", """",F4, """",", ", """",G4, """",", ", """",H4, """",", ", """",I4, """",", ", """",J4, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आओ मेरे सतगुरु हे मेरी जान", "Aao Mere Satguru He Meri Jan", "प्रेम बानी, भाग 1", "Prem Bani, Part - 1", "6", "1", "सत्संग आसाढ़ बदी पड़िवा, फ़र्याद एवं पुकार", "Satsang on Asadh Badi Padiwa , Invocation", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aao Mere Satguru He Meri Jan.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aao Mere Satguru He Meri Jan.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17376,7 +17378,7 @@
         <v>639</v>
       </c>
       <c r="K5" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A5, """",", ", """", B5, """",", ", """",C5, """",", ", """",D5, """",", ", """",E5, """",", ", """",F5, """",", ", """",G5, """",", ", """",H5, """",", ", """",I5, """",", ", """",J5, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "बार बार करूँ बीनती", "Bar Bar Karoon Binti", "प्रेम बानी, भाग 1", "Prem Bani, Part - 1", "6", "11", "मंगलाचरण एवं बिनती", "Manglacharan and Prayer", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Bar Bar Karoon Binti.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bar Bar Karoon Binti.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17412,7 +17414,7 @@
         <v>640</v>
       </c>
       <c r="K6" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A6, """",", ", """", B6, """",", ", """",C6, """",", ", """",D6, """",", ", """",E6, """",", ", """",F6, """",", ", """",G6, """",", ", """",H6, """",", ", """",I6, """",", ", """",J6, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज मेरे आनँद आनँद भारी", "Aaj Mere Anand Anand Bhari", "प्रेम बानी, भाग 1", "Prem Bani, Part - 1", "7", "3", "भंडारा महाराज साहब", "Bhandara of Maharaj Saheb", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Mere Anand Anand Bhari.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Mere Anand Anand Bhari.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17442,7 +17444,7 @@
         <v>641</v>
       </c>
       <c r="K7" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A7, """",", ", """", B7, """",", ", """",C7, """",", ", """",D7, """",", ", """",E7, """",", ", """",F7, """",", ", """",G7, """",", ", """",H7, """",", ", """",I7, """",", ", """",J7, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "परम पुरुष पूरन धनी", "Param Purush Pooran Dhani", "प्रेम बानी, भाग 1", "Prem Bani, Part - 1", "", "", "मंगलाचरण एवं बिनती", "Manglacharan and Prayer", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Param Purush Pooran Dhani.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Param Purush Pooran Dhani.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17478,7 +17480,7 @@
         <v>642</v>
       </c>
       <c r="K8" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A8, """",", ", """", B8, """",", ", """",C8, """",", ", """",D8, """",", ", """",E8, """",", ", """",F8, """",", ", """",G8, """",", ", """",H8, """",", ", """",I8, """",", ", """",J8, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "राधास्वामी चरन शीश मैं डारा", "Radhasoami Charan Shish Main Dara", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "10", "18", "आश्वासन एवं सांत्वना", "Assurance and solace ", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Radhasoami Charan Shish Main Dara.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Radhasoami Charan Shish Main Dara.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17514,7 +17516,7 @@
         <v>643</v>
       </c>
       <c r="K9" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A9, """",", ", """", B9, """",", ", """",C9, """",", ", """",D9, """",", ", """",E9, """",", ", """",F9, """",", ", """",G9, """",", ", """",H9, """",", ", """",I9, """",", ", """",J9, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज चलो बिदेसन अपने देश", "Aaj Chalo Bidesan Apne Desh", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "12", "3", "अंतिम समय एवं मृत्यु, नियमावली", "Illness and End Time or Death, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Chalo Bidesan Apne Desh.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Chalo Bidesan Apne Desh.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17550,7 +17552,7 @@
         <v>644</v>
       </c>
       <c r="K10" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A10, """",", ", """", B10, """",", ", """",C10, """",", ", """",D10, """",", ", """",E10, """",", ", """",F10, """",", ", """",G10, """",", ", """",H10, """",", ", """",I10, """",", ", """",J10, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज चलो पियारी अपने घर", "Aaj Chalo Piyari Apne Ghar", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "12", "4", "अंतिम समय एवं मृत्यु", "Illness and End Time or Death ", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Chalo Piyari Apne Ghar.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Chalo Piyari Apne Ghar.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17586,7 +17588,7 @@
         <v>645</v>
       </c>
       <c r="K11" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A11, """",", ", """", B11, """",", ", """",C11, """",", ", """",D11, """",", ", """",E11, """",", ", """",F11, """",", ", """",G11, """",", ", """",H11, """",", ", """",I11, """",", ", """",J11, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज पकड़ो गुरु के चरन सम्हार", "Aaj Pakado Guru Ke Charan Samhar", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "12", "9", "अंतिम समय एवं मृत्यु, नियमावली", "Illness and End Time or Death, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Pakado Guru Ke Charan Samhar.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Pakado Guru Ke Charan Samhar.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17622,7 +17624,7 @@
         <v>646</v>
       </c>
       <c r="K12" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A12, """",", ", """", B12, """",", ", """",C12, """",", ", """",D12, """",", ", """",E12, """",", ", """",F12, """",", ", """",G12, """",", ", """",H12, """",", ", """",I12, """",", ", """",J12, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज खेले सुरत गुरु चरनन पास", "Aaj Khele Surat Guru Charnan Pas", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "12", "36", "अंतिम समय एवं मृत्यु, नियमावली", "Illness and End Time or Death, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Khele Surat Guru Charnan Pas.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Khele Surat Guru Charnan Pas.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17658,7 +17660,7 @@
         <v>647</v>
       </c>
       <c r="K13" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A13, """",", ", """", B13, """",", ", """",C13, """",", ", """",D13, """",", ", """",E13, """",", ", """",F13, """",", ", """",G13, """",", ", """",H13, """",", ", """",I13, """",", ", """",J13, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "निज घर अपने चाल री मेरी प्यारी सुरतिया", "Nij Ghar Apne Chal Ri Meri Pyari Suratiya", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "12", "73", "अंतिम समय एवं मृत्यु", "Illness and End Time or Death ", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Nij Ghar Apne Chal Ri Meri Pyari Suratiya.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Nij Ghar Apne Chal Ri Meri Pyari Suratiya.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17694,7 +17696,7 @@
         <v>648</v>
       </c>
       <c r="K14" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A14, """",", ", """", B14, """",", ", """",C14, """",", ", """",D14, """",", ", """",E14, """",", ", """",F14, """",", ", """",G14, """",", ", """",H14, """",", ", """",I14, """",", ", """",J14, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज घिर आए बादल कारे", "Aaj Ghir Aaye Badal Kare", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "13", "27", "सावन, हिंडोला एवं झूला", "Sawan, Hindola and Jhula (Swing)", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Ghir Aaye Badal Kare.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Ghir Aaye Badal Kare.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17730,7 +17732,7 @@
         <v>649</v>
       </c>
       <c r="K15" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A15, """",", ", """", B15, """",", ", """",C15, """",", ", """",D15, """",", ", """",E15, """",", ", """",F15, """",", ", """",G15, """",", ", """",H15, """",", ", """",I15, """",", ", """",J15, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज बरसत रिमझिम मेघा कारे", "Aaj Barsat Rimjhim Megha Kare", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "13", "28", "सावन, हिंडोला एवं झूला", "Sawan, Hindola and Jhula (Swing)", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Barsat Rimjhim Megha Kare.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Barsat Rimjhim Megha Kare.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17766,7 +17768,7 @@
         <v>650</v>
       </c>
       <c r="K16" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A16, """",", ", """", B16, """",", ", """",C16, """",", ", """",D16, """",", ", """",E16, """",", ", """",F16, """",", ", """",G16, """",", ", """",H16, """",", ", """",I16, """",", ", """",J16, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "छबीले छवि लगे तोरी प्यारी", "Chhabile Chhavi Lage Tori Pyari", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "15", "1", "सत्संग गुरु पूर्णिमा", "Guru Purnima Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Chhabile Chhavi Lage Tori Pyari.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Chhabile Chhavi Lage Tori Pyari.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17802,7 +17804,7 @@
         <v>651</v>
       </c>
       <c r="K17" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A17, """",", ", """", B17, """",", ", """",C17, """",", ", """",D17, """",", ", """",E17, """",", ", """",F17, """",", ", """",G17, """",", ", """",H17, """",", ", """",I17, """",", ", """",J17, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "रँगीले रँग देओ चुनर हमारी", "Rangile Rang Deo Chunar Hamari", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "15", "2", "सत्संग गुरु पूर्णिमा", "Guru Purnima Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Rangile Rang Deo Chunar Hamari.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Rangile Rang Deo Chunar Hamari.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17838,7 +17840,7 @@
         <v>652</v>
       </c>
       <c r="K18" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A18, """",", ", """", B18, """",", ", """",C18, """",", ", """",D18, """",", ", """",E18, """",", ", """",F18, """",", ", """",G18, """",", ", """",H18, """",", ", """",I18, """",", ", """",J18, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "दया गुरु क्या करुँ वर्णन", "Daya Guru Kya Karoon Varnan", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "15", "16", "प्रार्थना दया एवं मेहर के लिये", "Prayer for Daya and Mehar", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Daya Guru Kya Karoon Varnan.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Daya Guru Kya Karoon Varnan.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17874,7 +17876,7 @@
         <v>653</v>
       </c>
       <c r="K19" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A19, """",", ", """", B19, """",", ", """",C19, """",", ", """",D19, """",", ", """",E19, """",", ", """",F19, """",", ", """",G19, """",", ", """",H19, """",", ", """",I19, """",", ", """",J19, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "गुरु प्यारे के दर्शन करत रहूँ", "Guru Pyare Ke Darshan Karat Rahoon", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "17", "17", "फ़र्याद एवं पुकार", "Invocation", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Guru Pyare Ke Darshan Karat Rahoon.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ke Darshan Karat Rahoon.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17910,7 +17912,7 @@
         <v>654</v>
       </c>
       <c r="K20" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A20, """",", ", """", B20, """",", ", """",C20, """",", ", """",D20, """",", ", """",E20, """",", ", """",F20, """",", ", """",G20, """",", ", """",H20, """",", ", """",I20, """",", ", """",J20, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "गुरु प्यारे के सँग प्यारी खेलो फाग", "Guru Pyare Ke Sang Pyari Khelo Phaag", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "17", "58", "होली सत्संग", "Holi Satang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Guru Pyare Ke Sang Pyari Khelo Phaag.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ke Sang Pyari Khelo Phaag.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17946,7 +17948,7 @@
         <v>655</v>
       </c>
       <c r="K21" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A21, """",", ", """", B21, """",", ", """",C21, """",", ", """",D21, """",", ", """",E21, """",", ", """",F21, """",", ", """",G21, """",", ", """",H21, """",", ", """",I21, """",", ", """",J21, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "गुरु प्यारे की मौज रहो तुम धार", "Guru Pyare Ki Mauj Raho Tum Dhar", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "17", "74", "आश्वासन एवं सांत्वना", "Assurance and solace ", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Guru Pyare Ki Mauj Raho Tum Dhar.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ki Mauj Raho Tum Dhar.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17982,7 +17984,7 @@
         <v>656</v>
       </c>
       <c r="K22" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A22, """",", ", """", B22, """",", ", """",C22, """",", ", """",D22, """",", ", """",E22, """",", ", """",F22, """",", ", """",G22, """",", ", """",H22, """",", ", """",I22, """",", ", """",J22, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "गुरु प्यारे का रँग चटकीला कभी उतरे नाहिं", "Guru Pyare Ka Rang Chatakila Kabhi Utre Nahin", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "18", "5", "सत्संग गुरु पूर्णिमा", "Guru Purnima Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Guru Pyare Ka Rang Chatakila Kabhi Utre Nahin.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ka Rang Chatakila Kabhi Utre Nahin.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18018,7 +18020,7 @@
         <v>657</v>
       </c>
       <c r="K23" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A23, """",", ", """", B23, """",", ", """",C23, """",", ", """",D23, """",", ", """",E23, """",", ", """",F23, """",", ", """",G23, """",", ", """",H23, """",", ", """",I23, """",", ", """",J23, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "गुरु प्यारे का रंग अति निरमल", "Guru Pyare Ka Rang Ati Nirmal", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "18", "6", "सत्संग गुरु पूर्णिमा", "Guru Purnima Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Guru Pyare Ka Rang Ati Nirmal.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ka Rang Ati Nirmal.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18054,7 +18056,7 @@
         <v>658</v>
       </c>
       <c r="K24" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A24, """",", ", """", B24, """",", ", """",C24, """",", ", """",D24, """",", ", """",E24, """",", ", """",F24, """",", ", """",G24, """",", ", """",H24, """",", ", """",I24, """",", ", """",J24, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "मेरे हिये में बजत बधाई संत सँग पाया रे", "Mere Hiye Mein Bajat Badhaee Sant Sang Paya Re", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "21", "1", "बधावा एवं शुकराना, नियमावली", "Thanksgiving, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Mere Hiye Mein Bajat Badhaee Sant Sang Paya Re.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Mere Hiye Mein Bajat Badhaee Sant Sang Paya Re.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18090,7 +18092,7 @@
         <v>659</v>
       </c>
       <c r="K25" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A25, """",", ", """", B25, """",", ", """",C25, """",", ", """",D25, """",", ", """",E25, """",", ", """",F25, """",", ", """",G25, """",", ", """",H25, """",", ", """",I25, """",", ", """",J25, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "कस प्रीतम से जाय मिलूँ मैं", "Kas Preetam Se Jay Miloon Main", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "21", "5", "प्रेम एवं विरह", "Love and Yearning", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Kas Preetam Se Jay Miloon Main.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Kas Preetam Se Jay Miloon Main.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18126,7 +18128,7 @@
         <v>660</v>
       </c>
       <c r="K26" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A26, """",", ", """", B26, """",", ", """",C26, """",", ", """",D26, """",", ", """",E26, """",", ", """",F26, """",", ", """",G26, """",", ", """",H26, """",", ", """",I26, """",", ", """",J26, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "जब से मैं देखा राधास्वामी का मुखड़ा", "Jab Se Main Dekha Radhasoami Ka Mukhada", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "24", "4", "अंतिम समय एवं मृत्यु, नियमावली", "Illness and End Time or Death, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Jab Se Main Dekha Radhasoami Ka Mukhada.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jab Se Main Dekha Radhasoami Ka Mukhada.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18162,7 +18164,7 @@
         <v>661</v>
       </c>
       <c r="K27" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A27, """",", ", """", B27, """",", ", """",C27, """",", ", """",D27, """",", ", """",E27, """",", ", """",F27, """",", ", """",G27, """",", ", """",H27, """",", ", """",I27, """",", ", """",J27, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "चल खेलिये सतगुरु से रंग होली आज सखी री", "Chal Kheliye Satguru Se Rang Holi Aaj Sakhi Ri", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "30", "5", "होली सत्संग", "Holi Satang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Chal Kheliye Satguru Se Rang Holi Aaj Sakhi Ri.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Chal Kheliye Satguru Se Rang Holi Aaj Sakhi Ri.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18198,7 +18200,7 @@
         <v>662</v>
       </c>
       <c r="K28" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A28, """",", ", """", B28, """",", ", """",C28, """",", ", """",D28, """",", ", """",E28, """",", ", """",F28, """",", ", """",G28, """",", ", """",H28, """",", ", """",I28, """",", ", """",J28, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "तुम सोचो अपने मन में या जग में दुक्ख घनेरा", "Tum Socho Apne Man Mein Ya Jag Mein Dukkh Ghanera", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "30", "10", "चितावनी", "Admonition", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Tum Socho Apne Man Mein Ya Jag Mein Dukkh Ghanera.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Tum Socho Apne Man Mein Ya Jag Mein Dukkh Ghanera.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18231,7 +18233,7 @@
         <v>663</v>
       </c>
       <c r="K29" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A29, """",", ", """", B29, """",", ", """",C29, """",", ", """",D29, """",", ", """",E29, """",", ", """",F29, """",", ", """",G29, """",", ", """",H29, """",", ", """",I29, """",", ", """",J29, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज आई बहार बसन्त", "Aaj Aayee Bahar Basant", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "36", "", "बसंत पंचमी सत्संग", "Basant Panchmi Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Aaee Bahar Basant.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Aayee Bahar Basant.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18264,7 +18266,7 @@
         <v>664</v>
       </c>
       <c r="K30" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A30, """",", ", """", B30, """",", ", """",C30, """",", ", """",D30, """",", ", """",E30, """",", ", """",F30, """",", ", """",G30, """",", ", """",H30, """",", ", """",I30, """",", ", """",J30, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज सँग सतगुरु खेलूँगी होरी", "Aaj Sang Satguru Kheloongi Hori", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "36", "", "होली सत्संग", "Holi Satang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Sang Satguru Kheloongi Hori.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Sang Satguru Kheloongi Hori.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18297,7 +18299,7 @@
         <v>665</v>
       </c>
       <c r="K31" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A31, """",", ", """", B31, """",", ", """",C31, """",", ", """",D31, """",", ", """",E31, """",", ", """",F31, """",", ", """",G31, """",", ", """",H31, """",", ", """",I31, """",", ", """",J31, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज आया बसन्त नवीन", "Aaj Aaya Basant Naveen", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "36", "", "बसंत पंचमी सत्संग", "Basant Panchmi Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Aaya Basant Naveen.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Aaya Basant Naveen.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18333,7 +18335,7 @@
         <v>666</v>
       </c>
       <c r="K32" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A32, """",", ", """", B32, """",", ", """",C32, """",", ", """",D32, """",", ", """",E32, """",", ", """",F32, """",", ", """",G32, """",", ", """",H32, """",", ", """",I32, """",", ", """",J32, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "तड़पत रही बेहाल दरस बिन मन नहिं माने", "Tadapat Rahi Behal Daras Bin Man Nahin Mane", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "37", "3", "प्रेम एवं विरह", "Love and Yearning", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Tadapat Rahi Behal Daras Bin Man Nahin Mane.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Tadapat Rahi Behal Daras Bin Man Nahin Mane.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18366,7 +18368,7 @@
         <v>667</v>
       </c>
       <c r="K33" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A33, """",", ", """", B33, """",", ", """",C33, """",", ", """",D33, """",", ", """",E33, """",", ", """",F33, """",", ", """",G33, """",", ", """",H33, """",", ", """",I33, """",", ", """",J33, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज आनन्द रहा मौज से चहुँ दिस छाई", "Aaj Anand Raha Mauj Se Chahun Dis Chhaee", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "39", "", "शादी व अन्य खुशी के मौके", "Marriage and Other Happy Occasions", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Anand Raha Mauj Se Chahun Dis Chhaee.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Anand Raha Mauj Se Chahun Dis Chhaee.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18399,7 +18401,7 @@
         <v>668</v>
       </c>
       <c r="K34" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A34, """",", ", """", B34, """",", ", """",C34, """",", ", """",D34, """",", ", """",E34, """",", ", """",F34, """",", ", """",G34, """",", ", """",H34, """",", ", """",I34, """",", ", """",J34, """"," ]")</f>
+        <f t="shared" ref="K34:K65" si="1">_xlfn.CONCAT("[ ", """", A34, """",", ", """", B34, """",", ", """",C34, """",", ", """",D34, """",", ", """",E34, """",", ", """",F34, """",", ", """",G34, """",", ", """",H34, """",", ", """",I34, """",", ", """",J34, """"," ]")</f>
         <v>[ "आज हंगामये शादी का गरम हो रहा देखो हर जा", "Aaj Hangamaye Shadi Ka Garam Ho Raha Dekho Har Ja", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "39", "", "शादी व अन्य खुशी के मौके", "Marriage and Other Happy Occasions", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Hangamaye Shadi Ka Garam Ho Raha Dekho Har Ja.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Hangamaye Shadi Ka Garam Ho Raha Dekho Har Ja.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18432,7 +18434,7 @@
         <v>669</v>
       </c>
       <c r="K35" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A35, """",", ", """", B35, """",", ", """",C35, """",", ", """",D35, """",", ", """",E35, """",", ", """",F35, """",", ", """",G35, """",", ", """",H35, """",", ", """",I35, """",", ", """",J35, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "आज गुरु प्यारे के चरनों में झलकती है", "Aaj Guru Pyare Ke Charnon Mein Jhalakati Hai", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "39", "", "शादी व अन्य खुशी के मौके", "Marriage and Other Happy Occasions", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Guru Pyare Ke Charnon Mein Jhalakati Hai.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Guru Pyare Ke Charnon Mein Jhalakati Hai.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18465,7 +18467,7 @@
         <v>670</v>
       </c>
       <c r="K36" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A36, """",", ", """", B36, """",", ", """",C36, """",", ", """",D36, """",", ", """",E36, """",", ", """",F36, """",", ", """",G36, """",", ", """",H36, """",", ", """",I36, """",", ", """",J36, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "जुड़ मिल के हंस सारे दर्शन को गुरु के आये", "Jud Mil Ke Hans Sare Darshan Ko Guru Ke Aaye", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "39", "", "गृह प्रवेश", "House warming", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Jud Mil Ke Hans Sare Darshan Ko Guru Ke Aaye.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jud Mil Ke Hans Sare Darshan Ko Guru Ke Aaye.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18498,7 +18500,7 @@
         <v>671</v>
       </c>
       <c r="K37" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A37, """",", ", """", B37, """",", ", """",C37, """",", ", """",D37, """",", ", """",E37, """",", ", """",F37, """",", ", """",G37, """",", ", """",H37, """",", ", """",I37, """",", ", """",J37, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "यह सतसंग और राधास्वामी है नाम", "Yeh Satsang Aur Radhasoami Hai Naam", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "39", "", "गज़ल एवं मसनवी", "Ghazal and Masnavi", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Yeh Satsang Aur Radhasoami Hai Naam.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Yeh Satsang Aur Radhasoami Hai Naam.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18531,7 +18533,7 @@
         <v>672</v>
       </c>
       <c r="K38" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A38, """",", ", """", B38, """",", ", """",C38, """",", ", """",D38, """",", ", """",E38, """",", ", """",F38, """",", ", """",G38, """",", ", """",H38, """",", ", """",I38, """",", ", """",J38, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "अहो मेरे सतगुरु अहो मेरी जान", "Aho Mere Satguru Aho Meri Jan", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "39", "", "बिनती एवं प्रार्थना, नियमावली", "Prayer, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aho Mere Satguru Aho Meri Jan.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aho Mere Satguru Aho Meri Jan.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18564,7 +18566,7 @@
         <v>673</v>
       </c>
       <c r="K39" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A39, """",", ", """", B39, """",", ", """",C39, """",", ", """",D39, """",", ", """",E39, """",", ", """",F39, """",", ", """",G39, """",", ", """",H39, """",", ", """",I39, """",", ", """",J39, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "जब देखा तेज मैंने जो मालिक के नाम का", "Jab Dekha Tej Maine Jo Malik Ke Naam Ka", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "39", "", "गज़ल एवं मसनवी", "Ghazal and Masnavi", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Jab Dekha Tej Maine Jo Malik Ke Naam Ka.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jab Dekha Tej Maine Jo Malik Ke Naam Ka.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18597,7 +18599,7 @@
         <v>674</v>
       </c>
       <c r="K40" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A40, """",", ", """", B40, """",", ", """",C40, """",", ", """",D40, """",", ", """",E40, """",", ", """",F40, """",", ", """",G40, """",", ", """",H40, """",", ", """",I40, """",", ", """",J40, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "बड़ा ज़ुल्म है मेरे यार", "Bada Julm Hai Mere Yar", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "39", "", "गज़ल एवं मसनवी", "Ghazal and Masnavi", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Bada Julm Hai Mere Yar.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bada Julm Hai Mere Yar.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18633,7 +18635,7 @@
         <v>675</v>
       </c>
       <c r="K41" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A41, """",", ", """", B41, """",", ", """",C41, """",", ", """",D41, """",", ", """",E41, """",", ", """",F41, """",", ", """",G41, """",", ", """",H41, """",", ", """",I41, """",", ", """",J41, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "क्यों सोच करे मन मूरख", "Kyon Soch Kare Man Moorakh", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "6", "आश्वासन एवं सांत्वना, नियमावली", "Assurance and solace, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Kyon Soch Kare Man Moorakh.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Kyon Soch Kare Man Moorakh.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18669,7 +18671,7 @@
         <v>676</v>
       </c>
       <c r="K42" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A42, """",", ", """", B42, """",", ", """",C42, """",", ", """",D42, """",", ", """",E42, """",", ", """",F42, """",", ", """",G42, """",", ", """",H42, """",", ", """",I42, """",", ", """",J42, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "अचरज आरत गुरु की धारूँ", "Achraj Aarat Guru Ki Dharoon", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "16", "भंडारा हुज़ूर महाराज", "Bhandara of Huzur Maharaj", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Achraj Aarat Guru Ki Dharoon.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Achraj Aarat Guru Ki Dharoon.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18705,7 +18707,7 @@
         <v>677</v>
       </c>
       <c r="K43" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A43, """",", ", """", B43, """",", ", """",C43, """",", ", """",D43, """",", ", """",E43, """",", ", """",F43, """",", ", """",G43, """",", ", """",H43, """",", ", """",I43, """",", ", """",J43, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "भागो रे जग से अब भागो", "Bhago Re Jag Se Ab Bhago", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "30", "चितावनी", "Admonition", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Bhago Re Jag Se Ab Bhago.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bhago Re Jag Se Ab Bhago.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18741,7 +18743,7 @@
         <v>678</v>
       </c>
       <c r="K44" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A44, """",", ", """", B44, """",", ", """",C44, """",", ", """",D44, """",", ", """",E44, """",", ", """",F44, """",", ", """",G44, """",", ", """",H44, """",", ", """",I44, """",", ", """",J44, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "चेतो रे घर घाट सम्हारो", "Cheto Re Ghar Ghat Samharo", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "31", "चितावनी", "Admonition", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Cheto Re Ghar Ghat Samharo.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Cheto Re Ghar Ghat Samharo.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18777,7 +18779,7 @@
         <v>679</v>
       </c>
       <c r="K45" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A45, """",", ", """", B45, """",", ", """",C45, """",", ", """",D45, """",", ", """",E45, """",", ", """",F45, """",", ", """",G45, """",", ", """",H45, """",", ", """",I45, """",", ", """",J45, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "जागो रे यहाँ कब लग सोना", "Jago Re Yehan Kab Lag Sona", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "32", "चितावनी", "Admonition", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Jago Re Yehan Kab Lag Sona.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jago Re Yehan Kab Lag Sona.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18813,7 +18815,7 @@
         <v>680</v>
       </c>
       <c r="K46" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A46, """",", ", """", B46, """",", ", """",C46, """",", ", """",D46, """",", ", """",E46, """",", ", """",F46, """",", ", """",G46, """",", ", """",H46, """",", ", """",I46, """",", ", """",J46, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "प्रेम दात गुरु दीजिये मेरे समरथ दाता हो", "Prem Dat Guru Dijiye Mere Samrath Data Ho", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "60", "फ़र्याद एवं पुकार, नियमावली", "Invocation, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Prem Dat Guru Dijiye Mere Samrath Data Ho.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Prem Dat Guru Dijiye Mere Samrath Data Ho.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18849,7 +18851,7 @@
         <v>681</v>
       </c>
       <c r="K47" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A47, """",", ", """", B47, """",", ", """",C47, """",", ", """",D47, """",", ", """",E47, """",", ", """",F47, """",", ", """",G47, """",", ", """",H47, """",", ", """",I47, """",", ", """",J47, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "हे मेरे समरथ साईं निज रूप दिखाओ", "He Mere Samarath Saeen Nij Roop Dikhao", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "80", "प्रेम एवं विरह", "Love and Yearning", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/He Mere Samarath Saeen Nij Roop Dikhao.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/He Mere Samarath Saeen Nij Roop Dikhao.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18885,7 +18887,7 @@
         <v>682</v>
       </c>
       <c r="K48" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A48, """",", ", """", B48, """",", ", """",C48, """",", ", """",D48, """",", ", """",E48, """",", ", """",F48, """",", ", """",G48, """",", ", """",H48, """",", ", """",I48, """",", ", """",J48, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "जो मेरे प्रीतम से प्रीत करे", "Jo Mere Preetam Se Preet Kare", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "82", "फ़र्याद एवं पुकार", "Invocation", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Jo Mere Preetam Se Preet Kare.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jo Mere Preetam Se Preet Kare.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18921,7 +18923,7 @@
         <v>683</v>
       </c>
       <c r="K49" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A49, """",", ", """", B49, """",", ", """",C49, """",", ", """",D49, """",", ", """",E49, """",", ", """",F49, """",", ", """",G49, """",", ", """",H49, """",", ", """",I49, """",", ", """",J49, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "जगत जीव सब होली पूजें", "Jagat Jeev Sab Holi Poojen", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "84", "होली सत्संग", "Holi Satang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Jagat Jeev Sab Holi Poojen.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jagat Jeev Sab Holi Poojen.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18954,7 +18956,7 @@
         <v>684</v>
       </c>
       <c r="K50" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A50, """",", ", """", B50, """",", ", """",C50, """",", ", """",D50, """",", ", """",E50, """",", ", """",F50, """",", ", """",G50, """",", ", """",H50, """",", ", """",I50, """",", ", """",J50, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "राधास्वामी नाम जो गावे सो ही तरे", "Radhasoami Naam Jo Gave So Hi Tare", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "3", "", "मंगलाचरण एवं बिनती", "Manglacharan and Prayer", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Radhasoami Naam Jo Gave So Hi Tare.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Radhasoami Naam Jo Gave So Hi Tare.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18990,7 +18992,7 @@
         <v>685</v>
       </c>
       <c r="K51" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A51, """",", ", """", B51, """",", ", """",C51, """",", ", """",D51, """",", ", """",E51, """",", ", """",F51, """",", ", """",G51, """",", ", """",H51, """",", ", """",I51, """",", ", """",J51, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "आज बधावा राधास्वामी गाऊँ", "Aaj Badhawa Radhasoami Gaoon", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "4", "2", "बधावा एवं शुकराना", "Thanksgiving", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Badhawa Radhasoami Gaoon.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Badhawa Radhasoami Gaoon.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19026,7 +19028,7 @@
         <v>686</v>
       </c>
       <c r="K52" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A52, """",", ", """", B52, """",", ", """",C52, """",", ", """",D52, """",", ", """",E52, """",", ", """",F52, """",", ", """",G52, """",", ", """",H52, """",", ", """",I52, """",", ", """",J52, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "आज मेरे धूम भई है भारी", "Aaj Mere Dhoom Bhai Hai Bhari", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "4", "3", "शादी व अन्य खुशी के मौके", "Marriage and Other Happy Occasions", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Mere Dhoom Bhai Hai Bhari.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Mere Dhoom Bhai Hai Bhari.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19062,7 +19064,7 @@
         <v>687</v>
       </c>
       <c r="K53" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A53, """",", ", """", B53, """",", ", """",C53, """",", ", """",D53, """",", ", """",E53, """",", ", """",F53, """",", ", """",G53, """",", ", """",H53, """",", ", """",I53, """",", ", """",J53, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "आज साज कर आरत लाई", "Aaj Saj Kar Aarat Laee", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "6", "4", "भंडारा महाराज साहब, सत्संग आसाढ़ बदी पड़िवा", "Bhandara of Maharaj Saheb, Satsang on Asadh Badi Padiwa", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Saj Kar Aarat Laee.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Saj Kar Aarat Laee.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19098,7 +19100,7 @@
         <v>688</v>
       </c>
       <c r="K54" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A54, """",", ", """", B54, """",", ", """",C54, """",", ", """",D54, """",", ", """",E54, """",", ", """",F54, """",", ", """",G54, """",", ", """",H54, """",", ", """",I54, """",", ", """",J54, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "आनँद मंगल आज साज सब आरत लाई", "Anand Mangal Aaj Saj Sab Aarat Laee", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "6", "6", "भंडारा बाबूजी महाराज", "Bhandara of Babuji Maharaj", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Anand Mangal Aaj Saj Sab Aarat Laee.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Anand Mangal Aaj Saj Sab Aarat Laee.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19134,7 +19136,7 @@
         <v>689</v>
       </c>
       <c r="K55" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A55, """",", ", """", B55, """",", ", """",C55, """",", ", """",D55, """",", ", """",E55, """",", ", """",F55, """",", ", """",G55, """",", ", """",H55, """",", ", """",I55, """",", ", """",J55, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "करूँ आरती राधास्वामी तन मन सुरत लगाय", "Karoon Arti Radhasoami Tan Man Surat Lagay", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "6", "7", "भंडारा महाराज साहब, भंडारा बाबूजी महाराज, आरतियाँ राधाजी महाराज, सत्संग आसाढ़ बदी पड़िवा", "Bhandara of Maharaj Saheb, Bhandara of Babuji Maharaj, Arti of Radhaji Maharaj ", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Karoon Arti Radhasoami Tan Man Surat Lagay.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Karoon Arti Radhasoami Tan Man Surat Lagay.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19170,7 +19172,7 @@
         <v>690</v>
       </c>
       <c r="K56" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A56, """",", ", """", B56, """",", ", """",C56, """",", ", """",D56, """",", ", """",E56, """",", ", """",F56, """",", ", """",G56, """",", ", """",H56, """",", ", """",I56, """",", ", """",J56, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "आरत करूँ आज सतगुरु की", "Aarat Karoon Aaj Satguru Ki", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "6", "15", "भंडारा बुआजी महाराज", "Bhandara of Buaji Maharaj", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aarat Karoon Aaj Satguru Ki.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aarat Karoon Aaj Satguru Ki.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19206,7 +19208,7 @@
         <v>691</v>
       </c>
       <c r="K57" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A57, """",", ", """", B57, """",", ", """",C57, """",", ", """",D57, """",", ", """",E57, """",", ", """",F57, """",", ", """",G57, """",", ", """",H57, """",", ", """",I57, """",", ", """",J57, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "करूँ बीनती दोउ कर जोरी", "Karoon Binti Dou Kar Jori", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "7", "1", "मंगलाचरण एवं बिनती", "Manglacharan and Prayer", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Karoon Binti Dou Kar Jori.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Karoon Binti Dou Kar Jori.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19242,7 +19244,7 @@
         <v>692</v>
       </c>
       <c r="K58" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A58, """",", ", """", B58, """",", ", """",C58, """",", ", """",D58, """",", ", """",E58, """",", ", """",F58, """",", ", """",G58, """",", ", """",H58, """",", ", """",I58, """",", ", """",J58, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "आज मेरे आनँद होत अपार", "Aaj Mere Anand Hot Apar", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "8", "4", "भंडारा हुज़ूर महाराज", "Bhandara of Huzur Maharaj", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Mere Anand Hot Apar.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Mere Anand Hot Apar.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19278,7 +19280,7 @@
         <v>693</v>
       </c>
       <c r="K59" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A59, """",", ", """", B59, """",", ", """",C59, """",", ", """",D59, """",", ", """",E59, """",", ", """",F59, """",", ", """",G59, """",", ", """",H59, """",", ", """",I59, """",", ", """",J59, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "गुरु की कर हर दम पूजा", "Guru Ki Kar Har Dam Pooja", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "18", "2", "सत्संग गुरु पूर्णिमा", "Guru Purnima Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Guru Ki Kar Har Dam Pooja.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Ki Kar Har Dam Pooja.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19314,7 +19316,7 @@
         <v>694</v>
       </c>
       <c r="K60" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A60, """",", ", """", B60, """",", ", """",C60, """",", ", """",D60, """",", ", """",E60, """",", ", """",F60, """",", ", """",G60, """",", ", """",H60, """",", ", """",I60, """",", ", """",J60, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "दर्द दुखी मैं बिरहिन भारी", "Dard Dukhi Main Birahin Bhari", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "27", "2", "प्रेम एवं विरह", "Satsang on Asadh Badi Padiwa, Love and Yearning ", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Dard Dukhi Main Birahin Bhari.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Dard Dukhi Main Birahin Bhari.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19350,7 +19352,7 @@
         <v>695</v>
       </c>
       <c r="K61" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A61, """",", ", """", B61, """",", ", """",C61, """",", ", """",D61, """",", ", """",E61, """",", ", """",F61, """",", ", """",G61, """",", ", """",H61, """",", ", """",I61, """",", ", """",J61, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "पिया बिन कैसे जिऊँ मैं प्यारी", "Piya Bin Kaise Jioon Main Pyari", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "27", "4", "प्रेम एवं विरह", "Satsang on Asadh Badi Padiwa, Love and Yearning", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Piya Bin Kaise Jioon Main Pyari.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Piya Bin Kaise Jioon Main Pyari.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19386,7 +19388,7 @@
         <v>696</v>
       </c>
       <c r="K62" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A62, """",", ", """", B62, """",", ", """",C62, """",", ", """",D62, """",", ", """",E62, """",", ", """",F62, """",", ", """",G62, """",", ", """",H62, """",", ", """",I62, """",", ", """",J62, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "चुनर मेरी मैली भई", "Chunar Meri Maili Bhayee", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "27", "6", "प्रेम एवं विरह", "Love and Yearning", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Chunar Meri Maili Bhayee.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Chunar Meri Maili Bhayee.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19422,7 +19424,7 @@
         <v>697</v>
       </c>
       <c r="K63" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A63, """",", ", """", B63, """",", ", """",C63, """",", ", """",D63, """",", ", """",E63, """",", ", """",F63, """",", ", """",G63, """",", ", """",H63, """",", ", """",I63, """",", ", """",J63, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "आज घड़ी अति पावन भावन", "Aaj Ghadi Ati Pawan Bhavan", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "28", "4", "गृह प्रवेश", "House warming", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Ghadi Ati Pawan Bhavan.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Ghadi Ati Pawan Bhavan.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19458,7 +19460,7 @@
         <v>698</v>
       </c>
       <c r="K64" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A64, """",", ", """", B64, """",", ", """",C64, """",", ", """",D64, """",", ", """",E64, """",", ", """",F64, """",", ", """",G64, """",", ", """",H64, """",", ", """",I64, """",", ", """",J64, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "गुरु चरन गिरह मेरे आये", "Guru Charan Girah Mere Aaye", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "28", "5", "गृह प्रवेश", "House warming", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Guru Charan Girah Mere Aaye.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Charan Girah Mere Aaye.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19494,7 +19496,7 @@
         <v>699</v>
       </c>
       <c r="K65" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A65, """",", ", """", B65, """",", ", """",C65, """",", ", """",D65, """",", ", """",E65, """",", ", """",F65, """",", ", """",G65, """",", ", """",H65, """",", ", """",I65, """",", ", """",J65, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "कौन करे आरत सतगुरु की", "Kaun Kare Aarat Satguru Ki", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "28", "6", "सत्संग गुरु पूर्णिमा", "Guru Purnima Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Kaun Kare Aarat Satguru Ki.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Kaun Kare Aarat Satguru Ki.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19530,7 +19532,7 @@
         <v>700</v>
       </c>
       <c r="K66" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A66, """",", ", """", B66, """",", ", """",C66, """",", ", """",D66, """",", ", """",E66, """",", ", """",F66, """",", ", """",G66, """",", ", """",H66, """",", ", """",I66, """",", ", """",J66, """"," ]")</f>
+        <f t="shared" ref="K66:K97" si="2">_xlfn.CONCAT("[ ", """", A66, """",", ", """", B66, """",", ", """",C66, """",", ", """",D66, """",", ", """",E66, """",", ", """",F66, """",", ", """",G66, """",", ", """",H66, """",", ", """",I66, """",", ", """",J66, """"," ]")</f>
         <v>[ "गुरु मैं गुनहगार अति भारी", "Guru Main Gunahagar Ati Bhari", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "29", "3", "रात को सोने से पहले, नियमावली", "Before retiring to bed in evening, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Guru Main Gunahagar Ati Bhari.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Main Gunahagar Ati Bhari.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19563,7 +19565,7 @@
         <v>701</v>
       </c>
       <c r="K67" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A67, """",", ", """", B67, """",", ", """",C67, """",", ", """",D67, """",", ", """",E67, """",", ", """",F67, """",", ", """",G67, """",", ", """",H67, """",", ", """",I67, """",", ", """",J67, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "आरत गाऊँ पूरे गुरु की", "Aarat Gaoon Poore Guru Ki", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "30", "2", "", "Arti Shabd", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aarat Gaoon Poore Guru Ki.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aarat Gaoon Poore Guru Ki.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19596,7 +19598,7 @@
         <v>702</v>
       </c>
       <c r="K68" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A68, """",", ", """", B68, """",", ", """",C68, """",", ", """",D68, """",", ", """",E68, """",", ", """",F68, """",", ", """",G68, """",", ", """",H68, """",", ", """",I68, """",", ", """",J68, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "राधास्वामी राधास्वामी राधास्वामी गाऊँ", "Radhasoami Radhasoami Radhasoami Gaoon", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "30", "3", "", "Ari Shabd", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Radhasoami Radhasoami Radhasoami Gaoon.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Radhasoami Radhasoami Radhasoami Gaoon.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19629,7 +19631,7 @@
         <v>703</v>
       </c>
       <c r="K69" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A69, """",", ", """", B69, """",", ", """",C69, """",", ", """",D69, """",", ", """",E69, """",", ", """",F69, """",", ", """",G69, """",", ", """",H69, """",", ", """",I69, """",", ", """",J69, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "गाऊँ आरती लेकर थाली", "Gaoon Arti Lekar Thali", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "30", "5", "", "Arti Shabd", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Gaoon Arti Lekar Thali.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Gaoon Arti Lekar Thali.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19662,7 +19664,7 @@
         <v>704</v>
       </c>
       <c r="K70" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A70, """",", ", """", B70, """",", ", """",C70, """",", ", """",D70, """",", ", """",E70, """",", ", """",F70, """",", ", """",G70, """",", ", """",H70, """",", ", """",I70, """",", ", """",J70, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "आज आरती करूँ सुहावन", "Aaj Arti Karoon Suhawan", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "30", "18", "", "Arti Shabd", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Arti Karoon Suhawan.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Arti Karoon Suhawan.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19698,7 +19700,7 @@
         <v>705</v>
       </c>
       <c r="K71" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A71, """",", ", """", B71, """",", ", """",C71, """",", ", """",D71, """",", ", """",E71, """",", ", """",F71, """",", ", """",G71, """",", ", """",H71, """",", ", """",I71, """",", ", """",J71, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "अब मन आतुर दरस पुकारे", "Ab Man Aatur Daras Pukare", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "33", "1", "फ़र्याद एवं पुकार", "Invocation", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Ab Man Aatur Daras Pukare.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ab Man Aatur Daras Pukare.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19731,7 +19733,7 @@
         <v>706</v>
       </c>
       <c r="K72" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A72, """",", ", """", B72, """",", ", """",C72, """",", ", """",D72, """",", ", """",E72, """",", ", """",F72, """",", ", """",G72, """",", ", """",H72, """",", ", """",I72, """",", ", """",J72, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "अब मैं कौन कुमति उरझानी", "Ab Main Kaun Kumati Urjhani", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "33", "2", "", "invocation", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Ab Main Kaun Kumati Urjhani.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ab Main Kaun Kumati Urjhani.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19767,7 +19769,7 @@
         <v>707</v>
       </c>
       <c r="K73" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A73, """",", ", """", B73, """",", ", """",C73, """",", ", """",D73, """",", ", """",E73, """",", ", """",F73, """",", ", """",G73, """",", ", """",H73, """",", ", """",I73, """",", ", """",J73, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "करत हूँ पुकार आज सुनिये गुहार", "Karat Hoon Pukar Aaj Suniye Guhar", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "33", "3", "सुबह उठने के बाद, नियमावली", "After waking up in morning, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Karat Hoon Pukar Aaj Suniye Guhar.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Karat Hoon Pukar Aaj Suniye Guhar.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19803,7 +19805,7 @@
         <v>708</v>
       </c>
       <c r="K74" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A74, """",", ", """", B74, """",", ", """",C74, """",", ", """",D74, """",", ", """",E74, """",", ", """",F74, """",", ", """",G74, """",", ", """",H74, """",", ", """",I74, """",", ", """",J74, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "लगाओ मेरी नइया सतगुरु पार", "Lagao Meri Naiya Satguru Par", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "33", "20", "अंतिम समय एवं मृत्यु", "Illness and End Time or Death ", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Lagao Meri Naiya Satguru Par.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Lagao Meri Naiya Satguru Par.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19836,7 +19838,7 @@
         <v>709</v>
       </c>
       <c r="K75" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A75, """",", ", """", B75, """",", ", """",C75, """",", ", """",D75, """",", ", """",E75, """",", ", """",F75, """",", ", """",G75, """",", ", """",H75, """",", ", """",I75, """",", ", """",J75, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "धीरज धरना मत घबराना", "Dhiraj Dharana Mat Ghabrana", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "33", "", "भंडारा हुज़ूर महाराज, नियमावली", "Bhandara of Huzur Maharaj, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Dhiraj Dharana Mat Ghabrana.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Dhiraj Dharana Mat Ghabrana.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19872,7 +19874,7 @@
         <v>710</v>
       </c>
       <c r="K76" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A76, """",", ", """", B76, """",", ", """",C76, """",", ", """",D76, """",", ", """",E76, """",", ", """",F76, """",", ", """",G76, """",", ", """",H76, """",", ", """",I76, """",", ", """",J76, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "आज काज मेरे कीन्हे पूरे", "Aaj Kaj Mere Kinhe Poore", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "34", "2", "प्रार्थना दया एवं मेहर के लिये", "Prayer for Daya and Mehar", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Kaj Mere Kinhe Poore.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Kaj Mere Kinhe Poore.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19908,7 +19910,7 @@
         <v>711</v>
       </c>
       <c r="K77" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A77, """",", ", """", B77, """",", ", """",C77, """",", ", """",D77, """",", ", """",E77, """",", ", """",F77, """",", ", """",G77, """",", ", """",H77, """",", ", """",I77, """",", ", """",J77, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "आओ री सिमट हे सखियो", "Aao Ri Simat He Sakhiyo", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "34", "13", "प्रार्थना दया एवं मेहर के लिये", "Prayer for Daya and Mehar", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aao Ri Simat He Sakhiyo.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aao Ri Simat He Sakhiyo.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19944,7 +19946,7 @@
         <v>712</v>
       </c>
       <c r="K78" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A78, """",", ", """", B78, """",", ", """",C78, """",", ", """",D78, """",", ", """",E78, """",", ", """",F78, """",", ", """",G78, """",", ", """",H78, """",", ", """",I78, """",", ", """",J78, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "घट में खेलूँ अब बसन्त", "Ghat Mein Kheloon Ab Basant", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "39", "2", "बसंत पंचमी सत्संग", "Basant Panchmi Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Ghat Mein Kheloon Ab Basant.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ghat Mein Kheloon Ab Basant.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19980,7 +19982,7 @@
         <v>713</v>
       </c>
       <c r="K79" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A79, """",", ", """", B79, """",", ", """",C79, """",", ", """",D79, """",", ", """",E79, """",", ", """",F79, """",", ", """",G79, """",", ", """",H79, """",", ", """",I79, """",", ", """",J79, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "देखन चली बसंत अगम घर", "Dekhan Chali Basant Agam Ghar", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "39", "4", "बसंत पंचमी सत्संग", "Basant Panchmi Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Dekhan Chali Basant Agam Ghar.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Dekhan Chali Basant Agam Ghar.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -20016,7 +20018,7 @@
         <v>714</v>
       </c>
       <c r="K80" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A80, """",", ", """", B80, """",", ", """",C80, """",", ", """",D80, """",", ", """",E80, """",", ", """",F80, """",", ", """",G80, """",", ", """",H80, """",", ", """",I80, """",", ", """",J80, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "अब खेलत राधास्वामी सँग होरी", "Ab Khelat Radhasoami Sang Hori", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "39", "5", "होली सत्संग", "Holi Satang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Ab Khelat Radhasoami Sang Hori.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ab Khelat Radhasoami Sang Hori.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -20052,7 +20054,7 @@
         <v>715</v>
       </c>
       <c r="K81" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A81, """",", ", """", B81, """",", ", """",C81, """",", ", """",D81, """",", ", """",E81, """",", ", """",F81, """",", ", """",G81, """",", ", """",H81, """",", ", """",I81, """",", ", """",J81, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "आओ री सखी जुड़ होली गावें", "Aao Ri Sakhi Jud Holi Gaven", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "39", "12", "होली सत्संग", "Holi Satang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aao Ri Sakhi Jud Holi Gaven.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aao Ri Sakhi Jud Holi Gaven.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -20088,7 +20090,7 @@
         <v>716</v>
       </c>
       <c r="K82" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A82, """",", ", """", B82, """",", ", """",C82, """",", ", """",D82, """",", ", """",E82, """",", ", """",F82, """",", ", """",G82, """",", ", """",H82, """",", ", """",I82, """",", ", """",J82, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "अजब यह बँगला लिया सजाय", "Ajab Yeh Bangla Liya Sajay", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "40", "5", "गृह प्रवेश", "House warming", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Ajab Yeh Bangla Liya Sajay.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ajab Yeh Bangla Liya Sajay.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -20124,7 +20126,7 @@
         <v>717</v>
       </c>
       <c r="K83" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A83, """",", ", """", B83, """",", ", """",C83, """",", ", """",D83, """",", ", """",E83, """",", ", """",F83, """",", ", """",G83, """",", ", """",H83, """",", ", """",I83, """",", ", """",J83, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "चौका बरतन किया अचंभी", "Chauka Bartan Kiya Achambhi", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "42", "2", "सेवा बानी", "Hyms of Sewa", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Chauka Bartan Kiya Achambhi.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Chauka Bartan Kiya Achambhi.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -20160,7 +20162,7 @@
         <v>718</v>
       </c>
       <c r="K84" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A84, """",", ", """", B84, """",", ", """",C84, """",", ", """",D84, """",", ", """",E84, """",", ", """",F84, """",", ", """",G84, """",", ", """",H84, """",", ", """",I84, """",", ", """",J84, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "भोग धरे राधास्वामी आगे", "Bhog Dhare Radhasoami Aage", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "42", "4", "भोग", "Bhog", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Bhog Dhare Radhasoami Aage.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bhog Dhare Radhasoami Aage.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Shabds by special occasions (#2)
</commit_message>
<xml_diff>
--- a/Video_Poetry.xlsx
+++ b/Video_Poetry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiki/Documents/Personal/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C907E024-2650-CC49-AC1C-2B25E8D45E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F9B1D9-35A0-7344-AEC4-6A17F2221C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22120" activeTab="2" xr2:uid="{8D838E60-7835-F44B-BD1C-2E58B2E8E6E1}"/>
   </bookViews>
@@ -7391,8 +7391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509C33A8-3102-F94A-82D6-D97CE7B00496}">
   <dimension ref="A1:P91"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="K1" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7465,7 +7465,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7519,7 +7519,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bar Bar Kar Jod Kar.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7573,7 +7573,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bhav Bhakti Se Binjan Karti.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>64</v>
       </c>
@@ -7627,7 +7627,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aao Mere Satguru He Meri Jan.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>74</v>
       </c>
@@ -7681,7 +7681,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bar Bar Karoon Binti.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>82</v>
       </c>
@@ -7735,7 +7735,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Mere Anand Anand Bhari.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>260</v>
       </c>
@@ -7789,7 +7789,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Param Purush Pooran Dhani.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>326</v>
       </c>
@@ -7843,7 +7843,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Radhasoami Charan Shish Main Dara.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>477</v>
       </c>
@@ -7897,7 +7897,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Chalo Bidesan Apne Desh.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>478</v>
       </c>
@@ -7951,7 +7951,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Chalo Piyari Apne Ghar.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>483</v>
       </c>
@@ -8005,7 +8005,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Pakado Guru Ke Charan Samhar.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>510</v>
       </c>
@@ -8059,7 +8059,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Khele Surat Guru Charnan Pas.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>547</v>
       </c>
@@ -8113,7 +8113,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Nij Ghar Apne Chal Ri Meri Pyari Suratiya.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>577</v>
       </c>
@@ -8167,7 +8167,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Ghir Aaye Badal Kare.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>578</v>
       </c>
@@ -8221,7 +8221,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Barsat Rimjhim Megha Kare.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>637</v>
       </c>
@@ -8275,7 +8275,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Chhabile Chhavi Lage Tori Pyari.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>638</v>
       </c>
@@ -8329,7 +8329,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Rangile Rang Deo Chunar Hamari.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>652</v>
       </c>
@@ -8383,7 +8383,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Daya Guru Kya Karoon Varnan.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>681</v>
       </c>
@@ -8437,7 +8437,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ke Darshan Karat Rahoon.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>722</v>
       </c>
@@ -8491,7 +8491,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ke Sang Pyari Khelo Phaag.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>738</v>
       </c>
@@ -8545,7 +8545,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ki Mauj Raho Tum Dhar.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>749</v>
       </c>
@@ -8599,7 +8599,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ka Rang Chatakila Kabhi Utre Nahin.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>750</v>
       </c>
@@ -8653,7 +8653,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ka Rang Ati Nirmal.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>841</v>
       </c>
@@ -8707,7 +8707,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Mere Hiye Mein Bajat Badhaee Sant Sang Paya Re.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>845</v>
       </c>
@@ -8761,7 +8761,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Kas Preetam Se Jay Miloon Main.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>865</v>
       </c>
@@ -8815,7 +8815,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jab Se Main Dekha Radhasoami Ka Mukhada.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>916</v>
       </c>
@@ -8869,7 +8869,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Chal Kheliye Satguru Se Rang Holi Aaj Sakhi Ri.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>921</v>
       </c>
@@ -8923,7 +8923,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Tum Socho Apne Man Mein Ya Jag Mein Dukkh Ghanera.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>947</v>
       </c>
@@ -8977,7 +8977,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Aayee Bahar Basant.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>970</v>
       </c>
@@ -9031,7 +9031,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Sang Satguru Kheloongi Hori.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>981</v>
       </c>
@@ -9085,7 +9085,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Aaya Basant Naveen.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>986</v>
       </c>
@@ -9139,7 +9139,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Tadapat Rahi Behal Daras Bin Man Nahin Mane.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1024</v>
       </c>
@@ -9193,7 +9193,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Anand Raha Mauj Se Chahun Dis Chhaee.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1025</v>
       </c>
@@ -9247,7 +9247,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Hangamaye Shadi Ka Garam Ho Raha Dekho Har Ja.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1026</v>
       </c>
@@ -9301,7 +9301,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Guru Pyare Ke Charnon Mein Jhalakati Hai.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1031</v>
       </c>
@@ -9355,7 +9355,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jud Mil Ke Hans Sare Darshan Ko Guru Ke Aaye.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1033</v>
       </c>
@@ -9409,7 +9409,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Yeh Satsang Aur Radhasoami Hai Naam.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1038</v>
       </c>
@@ -9463,7 +9463,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aho Mere Satguru Aho Meri Jan.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1039</v>
       </c>
@@ -9517,7 +9517,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jab Dekha Tej Maine Jo Malik Ke Naam Ka.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1046</v>
       </c>
@@ -9571,7 +9571,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bada Julm Hai Mere Yar.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1054</v>
       </c>
@@ -9625,7 +9625,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Kyon Soch Kare Man Moorakh.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1064</v>
       </c>
@@ -9679,7 +9679,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Achraj Aarat Guru Ki Dharoon.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1078</v>
       </c>
@@ -9733,7 +9733,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bhago Re Jag Se Ab Bhago.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1079</v>
       </c>
@@ -9787,7 +9787,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Cheto Re Ghar Ghat Samharo.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1080</v>
       </c>
@@ -9841,7 +9841,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jago Re Yehan Kab Lag Sona.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1108</v>
       </c>
@@ -9895,7 +9895,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Prem Dat Guru Dijiye Mere Samrath Data Ho.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1128</v>
       </c>
@@ -9949,7 +9949,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/He Mere Samarath Saeen Nij Roop Dikhao.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1130</v>
       </c>
@@ -10003,7 +10003,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jo Mere Preetam Se Preet Kare.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1132</v>
       </c>
@@ -10057,7 +10057,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jagat Jeev Sab Holi Poojen.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1263</v>
       </c>
@@ -10111,7 +10111,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Radhasoami Naam Jo Gave So Hi Tare.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1264</v>
       </c>
@@ -10165,7 +10165,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/NULLVIDEO'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1265</v>
       </c>
@@ -10219,7 +10219,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Badhawa Radhasoami Gaoon.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1266</v>
       </c>
@@ -10273,7 +10273,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Mere Dhoom Bhai Hai Bhari.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1280</v>
       </c>
@@ -10327,7 +10327,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Saj Kar Aarat Laee.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1282</v>
       </c>
@@ -10381,7 +10381,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Anand Mangal Aaj Saj Sab Aarat Laee.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1283</v>
       </c>
@@ -10435,7 +10435,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Karoon Arti Radhasoami Tan Man Surat Lagay.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1291</v>
       </c>
@@ -10489,7 +10489,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aarat Karoon Aaj Satguru Ki.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1301</v>
       </c>
@@ -10543,7 +10543,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Karoon Binti Dou Kar Jori.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1302</v>
       </c>
@@ -10594,7 +10594,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/NULLVIDEO'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1308</v>
       </c>
@@ -10648,7 +10648,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Mere Anand Hot Apar.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1382</v>
       </c>
@@ -10702,7 +10702,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Ki Kar Har Dam Pooja.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1383</v>
       </c>
@@ -10756,7 +10756,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/NULLVIDEO'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1475</v>
       </c>
@@ -10810,7 +10810,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Dard Dukhi Main Birahin Bhari.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1477</v>
       </c>
@@ -10864,7 +10864,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Piya Bin Kaise Jioon Main Pyari.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1479</v>
       </c>
@@ -10918,7 +10918,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Chunar Meri Maili Bhayee.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1484</v>
       </c>
@@ -10972,7 +10972,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Ghadi Ati Pawan Bhavan.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>1485</v>
       </c>
@@ -11026,7 +11026,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Charan Girah Mere Aaye.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>1486</v>
       </c>
@@ -11080,7 +11080,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Kaun Kare Aarat Satguru Ki.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1489</v>
       </c>
@@ -11134,7 +11134,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Main Gunahagar Ati Bhari.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1490</v>
       </c>
@@ -11182,7 +11182,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/NULLVIDEO'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1491</v>
       </c>
@@ -11233,7 +11233,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aarat Gaoon Poore Guru Ki.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1492</v>
       </c>
@@ -11284,7 +11284,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Radhasoami Radhasoami Radhasoami Gaoon.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1494</v>
       </c>
@@ -11335,7 +11335,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Gaoon Arti Lekar Thali.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1507</v>
       </c>
@@ -11386,7 +11386,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Arti Karoon Suhawan.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1529</v>
       </c>
@@ -11440,7 +11440,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ab Man Aatur Daras Pukare.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1530</v>
       </c>
@@ -11491,7 +11491,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ab Main Kaun Kumati Urjhani.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1531</v>
       </c>
@@ -11545,7 +11545,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Karat Hoon Pukar Aaj Suniye Guhar.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1532</v>
       </c>
@@ -11593,7 +11593,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/NULLVIDEO'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1548</v>
       </c>
@@ -11647,7 +11647,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Lagao Meri Naiya Satguru Par.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1553</v>
       </c>
@@ -11701,7 +11701,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Dhiraj Dharana Mat Ghabrana.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1554</v>
       </c>
@@ -11755,7 +11755,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/NULLVIDEO'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1555</v>
       </c>
@@ -11809,7 +11809,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Kaj Mere Kinhe Poore.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1566</v>
       </c>
@@ -11863,7 +11863,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aao Ri Simat He Sakhiyo.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1668</v>
       </c>
@@ -11917,7 +11917,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ghat Mein Kheloon Ab Basant.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1670</v>
       </c>
@@ -11971,7 +11971,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Dekhan Chali Basant Agam Ghar.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1671</v>
       </c>
@@ -12025,7 +12025,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ab Khelat Radhasoami Sang Hori.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1678</v>
       </c>
@@ -12079,7 +12079,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aao Ri Sakhi Jud Holi Gaven.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1683</v>
       </c>
@@ -12133,7 +12133,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ajab Yeh Bangla Liya Sajay.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1712</v>
       </c>
@@ -12187,7 +12187,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Chauka Bartan Kiya Achambhi.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>1714</v>
       </c>
@@ -12241,7 +12241,7 @@
         <v>&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bhog Dhare Radhasoami Aage.mp4'&gt;Video&lt;/a&gt;</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1715</v>
       </c>
@@ -12298,13 +12298,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D960A36-6FC1-8340-9C94-9BD4232780B8}">
   <dimension ref="A1:R91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:R91"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="17" width="10.83203125" style="4"/>
+    <col min="1" max="10" width="10.83203125" style="4"/>
+    <col min="11" max="16" width="39.6640625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="4"/>
     <col min="18" max="18" width="10.83203125" style="5"/>
     <col min="19" max="16384" width="10.83203125" style="4"/>
   </cols>
@@ -17274,7 +17276,7 @@
         <v>636</v>
       </c>
       <c r="K2" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A2, """",", ", """", B2, """",", ", """",C2, """",", ", """",D2, """",", ", """",E2, """",", ", """",F2, """",", ", """",G2, """",", ", """",H2, """",", ", """",I2, """",", ", """",J2, """"," ]")</f>
+        <f t="shared" ref="K2:K33" si="0">_xlfn.CONCAT("[ ", """", A2, """",", ", """", B2, """",", ", """",C2, """",", ", """",D2, """",", ", """",E2, """",", ", """",F2, """",", ", """",G2, """",", ", """",H2, """",", ", """",I2, """",", ", """",J2, """"," ]")</f>
         <v>[ "बार बार कर जोड़ कर", "Bar Bar Kar Jod Kar", "राधास्वामी मत पर प्रवचन", "Discourses on Radhasoami Faith", "", "1", "मंगलाचरण एवं बिनती", "Manglacharan and Prayer", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Bar Bar Kar Jod Kar.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bar Bar Kar Jod Kar.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17304,7 +17306,7 @@
         <v>637</v>
       </c>
       <c r="K3" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A3, """",", ", """", B3, """",", ", """",C3, """",", ", """",D3, """",", ", """",E3, """",", ", """",F3, """",", ", """",G3, """",", ", """",H3, """",", ", """",I3, """",", ", """",J3, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "भाव भक्ति से बिंजन करती", "Bhav Bhakti Se Binjan Karti", "नियमावली", "Sar Bachan Chand Band Part 2", "", "", "भोग, नियमावली", "Bhog, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Bhav Bhakti Se Binjan Karti.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bhav Bhakti Se Binjan Karti.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17340,7 +17342,7 @@
         <v>638</v>
       </c>
       <c r="K4" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A4, """",", ", """", B4, """",", ", """",C4, """",", ", """",D4, """",", ", """",E4, """",", ", """",F4, """",", ", """",G4, """",", ", """",H4, """",", ", """",I4, """",", ", """",J4, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आओ मेरे सतगुरु हे मेरी जान", "Aao Mere Satguru He Meri Jan", "प्रेम बानी, भाग 1", "Prem Bani, Part - 1", "6", "1", "सत्संग आसाढ़ बदी पड़िवा, फ़र्याद एवं पुकार", "Satsang on Asadh Badi Padiwa , Invocation", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aao Mere Satguru He Meri Jan.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aao Mere Satguru He Meri Jan.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17376,7 +17378,7 @@
         <v>639</v>
       </c>
       <c r="K5" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A5, """",", ", """", B5, """",", ", """",C5, """",", ", """",D5, """",", ", """",E5, """",", ", """",F5, """",", ", """",G5, """",", ", """",H5, """",", ", """",I5, """",", ", """",J5, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "बार बार करूँ बीनती", "Bar Bar Karoon Binti", "प्रेम बानी, भाग 1", "Prem Bani, Part - 1", "6", "11", "मंगलाचरण एवं बिनती", "Manglacharan and Prayer", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Bar Bar Karoon Binti.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bar Bar Karoon Binti.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17412,7 +17414,7 @@
         <v>640</v>
       </c>
       <c r="K6" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A6, """",", ", """", B6, """",", ", """",C6, """",", ", """",D6, """",", ", """",E6, """",", ", """",F6, """",", ", """",G6, """",", ", """",H6, """",", ", """",I6, """",", ", """",J6, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज मेरे आनँद आनँद भारी", "Aaj Mere Anand Anand Bhari", "प्रेम बानी, भाग 1", "Prem Bani, Part - 1", "7", "3", "भंडारा महाराज साहब", "Bhandara of Maharaj Saheb", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Mere Anand Anand Bhari.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Mere Anand Anand Bhari.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17442,7 +17444,7 @@
         <v>641</v>
       </c>
       <c r="K7" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A7, """",", ", """", B7, """",", ", """",C7, """",", ", """",D7, """",", ", """",E7, """",", ", """",F7, """",", ", """",G7, """",", ", """",H7, """",", ", """",I7, """",", ", """",J7, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "परम पुरुष पूरन धनी", "Param Purush Pooran Dhani", "प्रेम बानी, भाग 1", "Prem Bani, Part - 1", "", "", "मंगलाचरण एवं बिनती", "Manglacharan and Prayer", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Param Purush Pooran Dhani.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Param Purush Pooran Dhani.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17478,7 +17480,7 @@
         <v>642</v>
       </c>
       <c r="K8" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A8, """",", ", """", B8, """",", ", """",C8, """",", ", """",D8, """",", ", """",E8, """",", ", """",F8, """",", ", """",G8, """",", ", """",H8, """",", ", """",I8, """",", ", """",J8, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "राधास्वामी चरन शीश मैं डारा", "Radhasoami Charan Shish Main Dara", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "10", "18", "आश्वासन एवं सांत्वना", "Assurance and solace ", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Radhasoami Charan Shish Main Dara.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Radhasoami Charan Shish Main Dara.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17514,7 +17516,7 @@
         <v>643</v>
       </c>
       <c r="K9" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A9, """",", ", """", B9, """",", ", """",C9, """",", ", """",D9, """",", ", """",E9, """",", ", """",F9, """",", ", """",G9, """",", ", """",H9, """",", ", """",I9, """",", ", """",J9, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज चलो बिदेसन अपने देश", "Aaj Chalo Bidesan Apne Desh", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "12", "3", "अंतिम समय एवं मृत्यु, नियमावली", "Illness and End Time or Death, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Chalo Bidesan Apne Desh.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Chalo Bidesan Apne Desh.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17550,7 +17552,7 @@
         <v>644</v>
       </c>
       <c r="K10" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A10, """",", ", """", B10, """",", ", """",C10, """",", ", """",D10, """",", ", """",E10, """",", ", """",F10, """",", ", """",G10, """",", ", """",H10, """",", ", """",I10, """",", ", """",J10, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज चलो पियारी अपने घर", "Aaj Chalo Piyari Apne Ghar", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "12", "4", "अंतिम समय एवं मृत्यु", "Illness and End Time or Death ", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Chalo Piyari Apne Ghar.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Chalo Piyari Apne Ghar.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17586,7 +17588,7 @@
         <v>645</v>
       </c>
       <c r="K11" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A11, """",", ", """", B11, """",", ", """",C11, """",", ", """",D11, """",", ", """",E11, """",", ", """",F11, """",", ", """",G11, """",", ", """",H11, """",", ", """",I11, """",", ", """",J11, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज पकड़ो गुरु के चरन सम्हार", "Aaj Pakado Guru Ke Charan Samhar", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "12", "9", "अंतिम समय एवं मृत्यु, नियमावली", "Illness and End Time or Death, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Pakado Guru Ke Charan Samhar.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Pakado Guru Ke Charan Samhar.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17622,7 +17624,7 @@
         <v>646</v>
       </c>
       <c r="K12" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A12, """",", ", """", B12, """",", ", """",C12, """",", ", """",D12, """",", ", """",E12, """",", ", """",F12, """",", ", """",G12, """",", ", """",H12, """",", ", """",I12, """",", ", """",J12, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज खेले सुरत गुरु चरनन पास", "Aaj Khele Surat Guru Charnan Pas", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "12", "36", "अंतिम समय एवं मृत्यु, नियमावली", "Illness and End Time or Death, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Khele Surat Guru Charnan Pas.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Khele Surat Guru Charnan Pas.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17658,7 +17660,7 @@
         <v>647</v>
       </c>
       <c r="K13" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A13, """",", ", """", B13, """",", ", """",C13, """",", ", """",D13, """",", ", """",E13, """",", ", """",F13, """",", ", """",G13, """",", ", """",H13, """",", ", """",I13, """",", ", """",J13, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "निज घर अपने चाल री मेरी प्यारी सुरतिया", "Nij Ghar Apne Chal Ri Meri Pyari Suratiya", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "12", "73", "अंतिम समय एवं मृत्यु", "Illness and End Time or Death ", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Nij Ghar Apne Chal Ri Meri Pyari Suratiya.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Nij Ghar Apne Chal Ri Meri Pyari Suratiya.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17694,7 +17696,7 @@
         <v>648</v>
       </c>
       <c r="K14" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A14, """",", ", """", B14, """",", ", """",C14, """",", ", """",D14, """",", ", """",E14, """",", ", """",F14, """",", ", """",G14, """",", ", """",H14, """",", ", """",I14, """",", ", """",J14, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज घिर आए बादल कारे", "Aaj Ghir Aaye Badal Kare", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "13", "27", "सावन, हिंडोला एवं झूला", "Sawan, Hindola and Jhula (Swing)", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Ghir Aaye Badal Kare.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Ghir Aaye Badal Kare.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17730,7 +17732,7 @@
         <v>649</v>
       </c>
       <c r="K15" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A15, """",", ", """", B15, """",", ", """",C15, """",", ", """",D15, """",", ", """",E15, """",", ", """",F15, """",", ", """",G15, """",", ", """",H15, """",", ", """",I15, """",", ", """",J15, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज बरसत रिमझिम मेघा कारे", "Aaj Barsat Rimjhim Megha Kare", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "13", "28", "सावन, हिंडोला एवं झूला", "Sawan, Hindola and Jhula (Swing)", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Barsat Rimjhim Megha Kare.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Barsat Rimjhim Megha Kare.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17766,7 +17768,7 @@
         <v>650</v>
       </c>
       <c r="K16" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A16, """",", ", """", B16, """",", ", """",C16, """",", ", """",D16, """",", ", """",E16, """",", ", """",F16, """",", ", """",G16, """",", ", """",H16, """",", ", """",I16, """",", ", """",J16, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "छबीले छवि लगे तोरी प्यारी", "Chhabile Chhavi Lage Tori Pyari", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "15", "1", "सत्संग गुरु पूर्णिमा", "Guru Purnima Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Chhabile Chhavi Lage Tori Pyari.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Chhabile Chhavi Lage Tori Pyari.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17802,7 +17804,7 @@
         <v>651</v>
       </c>
       <c r="K17" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A17, """",", ", """", B17, """",", ", """",C17, """",", ", """",D17, """",", ", """",E17, """",", ", """",F17, """",", ", """",G17, """",", ", """",H17, """",", ", """",I17, """",", ", """",J17, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "रँगीले रँग देओ चुनर हमारी", "Rangile Rang Deo Chunar Hamari", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "15", "2", "सत्संग गुरु पूर्णिमा", "Guru Purnima Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Rangile Rang Deo Chunar Hamari.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Rangile Rang Deo Chunar Hamari.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17838,7 +17840,7 @@
         <v>652</v>
       </c>
       <c r="K18" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A18, """",", ", """", B18, """",", ", """",C18, """",", ", """",D18, """",", ", """",E18, """",", ", """",F18, """",", ", """",G18, """",", ", """",H18, """",", ", """",I18, """",", ", """",J18, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "दया गुरु क्या करुँ वर्णन", "Daya Guru Kya Karoon Varnan", "प्रेम बानी, भाग 2", "Prem Bani, Part - 2", "15", "16", "प्रार्थना दया एवं मेहर के लिये", "Prayer for Daya and Mehar", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Daya Guru Kya Karoon Varnan.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Daya Guru Kya Karoon Varnan.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17874,7 +17876,7 @@
         <v>653</v>
       </c>
       <c r="K19" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A19, """",", ", """", B19, """",", ", """",C19, """",", ", """",D19, """",", ", """",E19, """",", ", """",F19, """",", ", """",G19, """",", ", """",H19, """",", ", """",I19, """",", ", """",J19, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "गुरु प्यारे के दर्शन करत रहूँ", "Guru Pyare Ke Darshan Karat Rahoon", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "17", "17", "फ़र्याद एवं पुकार", "Invocation", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Guru Pyare Ke Darshan Karat Rahoon.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ke Darshan Karat Rahoon.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17910,7 +17912,7 @@
         <v>654</v>
       </c>
       <c r="K20" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A20, """",", ", """", B20, """",", ", """",C20, """",", ", """",D20, """",", ", """",E20, """",", ", """",F20, """",", ", """",G20, """",", ", """",H20, """",", ", """",I20, """",", ", """",J20, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "गुरु प्यारे के सँग प्यारी खेलो फाग", "Guru Pyare Ke Sang Pyari Khelo Phaag", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "17", "58", "होली सत्संग", "Holi Satang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Guru Pyare Ke Sang Pyari Khelo Phaag.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ke Sang Pyari Khelo Phaag.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17946,7 +17948,7 @@
         <v>655</v>
       </c>
       <c r="K21" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A21, """",", ", """", B21, """",", ", """",C21, """",", ", """",D21, """",", ", """",E21, """",", ", """",F21, """",", ", """",G21, """",", ", """",H21, """",", ", """",I21, """",", ", """",J21, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "गुरु प्यारे की मौज रहो तुम धार", "Guru Pyare Ki Mauj Raho Tum Dhar", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "17", "74", "आश्वासन एवं सांत्वना", "Assurance and solace ", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Guru Pyare Ki Mauj Raho Tum Dhar.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ki Mauj Raho Tum Dhar.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -17982,7 +17984,7 @@
         <v>656</v>
       </c>
       <c r="K22" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A22, """",", ", """", B22, """",", ", """",C22, """",", ", """",D22, """",", ", """",E22, """",", ", """",F22, """",", ", """",G22, """",", ", """",H22, """",", ", """",I22, """",", ", """",J22, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "गुरु प्यारे का रँग चटकीला कभी उतरे नाहिं", "Guru Pyare Ka Rang Chatakila Kabhi Utre Nahin", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "18", "5", "सत्संग गुरु पूर्णिमा", "Guru Purnima Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Guru Pyare Ka Rang Chatakila Kabhi Utre Nahin.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ka Rang Chatakila Kabhi Utre Nahin.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18018,7 +18020,7 @@
         <v>657</v>
       </c>
       <c r="K23" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A23, """",", ", """", B23, """",", ", """",C23, """",", ", """",D23, """",", ", """",E23, """",", ", """",F23, """",", ", """",G23, """",", ", """",H23, """",", ", """",I23, """",", ", """",J23, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "गुरु प्यारे का रंग अति निरमल", "Guru Pyare Ka Rang Ati Nirmal", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "18", "6", "सत्संग गुरु पूर्णिमा", "Guru Purnima Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Guru Pyare Ka Rang Ati Nirmal.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Pyare Ka Rang Ati Nirmal.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18054,7 +18056,7 @@
         <v>658</v>
       </c>
       <c r="K24" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A24, """",", ", """", B24, """",", ", """",C24, """",", ", """",D24, """",", ", """",E24, """",", ", """",F24, """",", ", """",G24, """",", ", """",H24, """",", ", """",I24, """",", ", """",J24, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "मेरे हिये में बजत बधाई संत सँग पाया रे", "Mere Hiye Mein Bajat Badhaee Sant Sang Paya Re", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "21", "1", "बधावा एवं शुकराना, नियमावली", "Thanksgiving, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Mere Hiye Mein Bajat Badhaee Sant Sang Paya Re.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Mere Hiye Mein Bajat Badhaee Sant Sang Paya Re.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18090,7 +18092,7 @@
         <v>659</v>
       </c>
       <c r="K25" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A25, """",", ", """", B25, """",", ", """",C25, """",", ", """",D25, """",", ", """",E25, """",", ", """",F25, """",", ", """",G25, """",", ", """",H25, """",", ", """",I25, """",", ", """",J25, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "कस प्रीतम से जाय मिलूँ मैं", "Kas Preetam Se Jay Miloon Main", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "21", "5", "प्रेम एवं विरह", "Love and Yearning", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Kas Preetam Se Jay Miloon Main.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Kas Preetam Se Jay Miloon Main.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18126,7 +18128,7 @@
         <v>660</v>
       </c>
       <c r="K26" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A26, """",", ", """", B26, """",", ", """",C26, """",", ", """",D26, """",", ", """",E26, """",", ", """",F26, """",", ", """",G26, """",", ", """",H26, """",", ", """",I26, """",", ", """",J26, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "जब से मैं देखा राधास्वामी का मुखड़ा", "Jab Se Main Dekha Radhasoami Ka Mukhada", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "24", "4", "अंतिम समय एवं मृत्यु, नियमावली", "Illness and End Time or Death, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Jab Se Main Dekha Radhasoami Ka Mukhada.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jab Se Main Dekha Radhasoami Ka Mukhada.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18162,7 +18164,7 @@
         <v>661</v>
       </c>
       <c r="K27" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A27, """",", ", """", B27, """",", ", """",C27, """",", ", """",D27, """",", ", """",E27, """",", ", """",F27, """",", ", """",G27, """",", ", """",H27, """",", ", """",I27, """",", ", """",J27, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "चल खेलिये सतगुरु से रंग होली आज सखी री", "Chal Kheliye Satguru Se Rang Holi Aaj Sakhi Ri", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "30", "5", "होली सत्संग", "Holi Satang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Chal Kheliye Satguru Se Rang Holi Aaj Sakhi Ri.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Chal Kheliye Satguru Se Rang Holi Aaj Sakhi Ri.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18198,7 +18200,7 @@
         <v>662</v>
       </c>
       <c r="K28" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A28, """",", ", """", B28, """",", ", """",C28, """",", ", """",D28, """",", ", """",E28, """",", ", """",F28, """",", ", """",G28, """",", ", """",H28, """",", ", """",I28, """",", ", """",J28, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "तुम सोचो अपने मन में या जग में दुक्ख घनेरा", "Tum Socho Apne Man Mein Ya Jag Mein Dukkh Ghanera", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "30", "10", "चितावनी", "Admonition", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Tum Socho Apne Man Mein Ya Jag Mein Dukkh Ghanera.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Tum Socho Apne Man Mein Ya Jag Mein Dukkh Ghanera.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18231,7 +18233,7 @@
         <v>663</v>
       </c>
       <c r="K29" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A29, """",", ", """", B29, """",", ", """",C29, """",", ", """",D29, """",", ", """",E29, """",", ", """",F29, """",", ", """",G29, """",", ", """",H29, """",", ", """",I29, """",", ", """",J29, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज आई बहार बसन्त", "Aaj Aayee Bahar Basant", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "36", "", "बसंत पंचमी सत्संग", "Basant Panchmi Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Aaee Bahar Basant.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Aayee Bahar Basant.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18264,7 +18266,7 @@
         <v>664</v>
       </c>
       <c r="K30" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A30, """",", ", """", B30, """",", ", """",C30, """",", ", """",D30, """",", ", """",E30, """",", ", """",F30, """",", ", """",G30, """",", ", """",H30, """",", ", """",I30, """",", ", """",J30, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज सँग सतगुरु खेलूँगी होरी", "Aaj Sang Satguru Kheloongi Hori", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "36", "", "होली सत्संग", "Holi Satang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Sang Satguru Kheloongi Hori.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Sang Satguru Kheloongi Hori.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18297,7 +18299,7 @@
         <v>665</v>
       </c>
       <c r="K31" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A31, """",", ", """", B31, """",", ", """",C31, """",", ", """",D31, """",", ", """",E31, """",", ", """",F31, """",", ", """",G31, """",", ", """",H31, """",", ", """",I31, """",", ", """",J31, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज आया बसन्त नवीन", "Aaj Aaya Basant Naveen", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "36", "", "बसंत पंचमी सत्संग", "Basant Panchmi Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Aaya Basant Naveen.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Aaya Basant Naveen.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18333,7 +18335,7 @@
         <v>666</v>
       </c>
       <c r="K32" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A32, """",", ", """", B32, """",", ", """",C32, """",", ", """",D32, """",", ", """",E32, """",", ", """",F32, """",", ", """",G32, """",", ", """",H32, """",", ", """",I32, """",", ", """",J32, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "तड़पत रही बेहाल दरस बिन मन नहिं माने", "Tadapat Rahi Behal Daras Bin Man Nahin Mane", "प्रेम बानी, भाग 3", "Prem Bani, Part - 3", "37", "3", "प्रेम एवं विरह", "Love and Yearning", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Tadapat Rahi Behal Daras Bin Man Nahin Mane.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Tadapat Rahi Behal Daras Bin Man Nahin Mane.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18366,7 +18368,7 @@
         <v>667</v>
       </c>
       <c r="K33" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A33, """",", ", """", B33, """",", ", """",C33, """",", ", """",D33, """",", ", """",E33, """",", ", """",F33, """",", ", """",G33, """",", ", """",H33, """",", ", """",I33, """",", ", """",J33, """"," ]")</f>
+        <f t="shared" si="0"/>
         <v>[ "आज आनन्द रहा मौज से चहुँ दिस छाई", "Aaj Anand Raha Mauj Se Chahun Dis Chhaee", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "39", "", "शादी व अन्य खुशी के मौके", "Marriage and Other Happy Occasions", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Anand Raha Mauj Se Chahun Dis Chhaee.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Anand Raha Mauj Se Chahun Dis Chhaee.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18399,7 +18401,7 @@
         <v>668</v>
       </c>
       <c r="K34" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A34, """",", ", """", B34, """",", ", """",C34, """",", ", """",D34, """",", ", """",E34, """",", ", """",F34, """",", ", """",G34, """",", ", """",H34, """",", ", """",I34, """",", ", """",J34, """"," ]")</f>
+        <f t="shared" ref="K34:K65" si="1">_xlfn.CONCAT("[ ", """", A34, """",", ", """", B34, """",", ", """",C34, """",", ", """",D34, """",", ", """",E34, """",", ", """",F34, """",", ", """",G34, """",", ", """",H34, """",", ", """",I34, """",", ", """",J34, """"," ]")</f>
         <v>[ "आज हंगामये शादी का गरम हो रहा देखो हर जा", "Aaj Hangamaye Shadi Ka Garam Ho Raha Dekho Har Ja", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "39", "", "शादी व अन्य खुशी के मौके", "Marriage and Other Happy Occasions", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Hangamaye Shadi Ka Garam Ho Raha Dekho Har Ja.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Hangamaye Shadi Ka Garam Ho Raha Dekho Har Ja.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18432,7 +18434,7 @@
         <v>669</v>
       </c>
       <c r="K35" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A35, """",", ", """", B35, """",", ", """",C35, """",", ", """",D35, """",", ", """",E35, """",", ", """",F35, """",", ", """",G35, """",", ", """",H35, """",", ", """",I35, """",", ", """",J35, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "आज गुरु प्यारे के चरनों में झलकती है", "Aaj Guru Pyare Ke Charnon Mein Jhalakati Hai", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "39", "", "शादी व अन्य खुशी के मौके", "Marriage and Other Happy Occasions", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Guru Pyare Ke Charnon Mein Jhalakati Hai.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Guru Pyare Ke Charnon Mein Jhalakati Hai.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18465,7 +18467,7 @@
         <v>670</v>
       </c>
       <c r="K36" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A36, """",", ", """", B36, """",", ", """",C36, """",", ", """",D36, """",", ", """",E36, """",", ", """",F36, """",", ", """",G36, """",", ", """",H36, """",", ", """",I36, """",", ", """",J36, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "जुड़ मिल के हंस सारे दर्शन को गुरु के आये", "Jud Mil Ke Hans Sare Darshan Ko Guru Ke Aaye", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "39", "", "गृह प्रवेश", "House warming", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Jud Mil Ke Hans Sare Darshan Ko Guru Ke Aaye.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jud Mil Ke Hans Sare Darshan Ko Guru Ke Aaye.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18498,7 +18500,7 @@
         <v>671</v>
       </c>
       <c r="K37" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A37, """",", ", """", B37, """",", ", """",C37, """",", ", """",D37, """",", ", """",E37, """",", ", """",F37, """",", ", """",G37, """",", ", """",H37, """",", ", """",I37, """",", ", """",J37, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "यह सतसंग और राधास्वामी है नाम", "Yeh Satsang Aur Radhasoami Hai Naam", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "39", "", "गज़ल एवं मसनवी", "Ghazal and Masnavi", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Yeh Satsang Aur Radhasoami Hai Naam.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Yeh Satsang Aur Radhasoami Hai Naam.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18531,7 +18533,7 @@
         <v>672</v>
       </c>
       <c r="K38" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A38, """",", ", """", B38, """",", ", """",C38, """",", ", """",D38, """",", ", """",E38, """",", ", """",F38, """",", ", """",G38, """",", ", """",H38, """",", ", """",I38, """",", ", """",J38, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "अहो मेरे सतगुरु अहो मेरी जान", "Aho Mere Satguru Aho Meri Jan", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "39", "", "बिनती एवं प्रार्थना, नियमावली", "Prayer, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aho Mere Satguru Aho Meri Jan.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aho Mere Satguru Aho Meri Jan.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18564,7 +18566,7 @@
         <v>673</v>
       </c>
       <c r="K39" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A39, """",", ", """", B39, """",", ", """",C39, """",", ", """",D39, """",", ", """",E39, """",", ", """",F39, """",", ", """",G39, """",", ", """",H39, """",", ", """",I39, """",", ", """",J39, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "जब देखा तेज मैंने जो मालिक के नाम का", "Jab Dekha Tej Maine Jo Malik Ke Naam Ka", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "39", "", "गज़ल एवं मसनवी", "Ghazal and Masnavi", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Jab Dekha Tej Maine Jo Malik Ke Naam Ka.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jab Dekha Tej Maine Jo Malik Ke Naam Ka.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18597,7 +18599,7 @@
         <v>674</v>
       </c>
       <c r="K40" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A40, """",", ", """", B40, """",", ", """",C40, """",", ", """",D40, """",", ", """",E40, """",", ", """",F40, """",", ", """",G40, """",", ", """",H40, """",", ", """",I40, """",", ", """",J40, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "बड़ा ज़ुल्म है मेरे यार", "Bada Julm Hai Mere Yar", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "39", "", "गज़ल एवं मसनवी", "Ghazal and Masnavi", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Bada Julm Hai Mere Yar.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bada Julm Hai Mere Yar.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18633,7 +18635,7 @@
         <v>675</v>
       </c>
       <c r="K41" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A41, """",", ", """", B41, """",", ", """",C41, """",", ", """",D41, """",", ", """",E41, """",", ", """",F41, """",", ", """",G41, """",", ", """",H41, """",", ", """",I41, """",", ", """",J41, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "क्यों सोच करे मन मूरख", "Kyon Soch Kare Man Moorakh", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "6", "आश्वासन एवं सांत्वना, नियमावली", "Assurance and solace, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Kyon Soch Kare Man Moorakh.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Kyon Soch Kare Man Moorakh.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18669,7 +18671,7 @@
         <v>676</v>
       </c>
       <c r="K42" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A42, """",", ", """", B42, """",", ", """",C42, """",", ", """",D42, """",", ", """",E42, """",", ", """",F42, """",", ", """",G42, """",", ", """",H42, """",", ", """",I42, """",", ", """",J42, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "अचरज आरत गुरु की धारूँ", "Achraj Aarat Guru Ki Dharoon", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "16", "भंडारा हुज़ूर महाराज", "Bhandara of Huzur Maharaj", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Achraj Aarat Guru Ki Dharoon.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Achraj Aarat Guru Ki Dharoon.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18705,7 +18707,7 @@
         <v>677</v>
       </c>
       <c r="K43" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A43, """",", ", """", B43, """",", ", """",C43, """",", ", """",D43, """",", ", """",E43, """",", ", """",F43, """",", ", """",G43, """",", ", """",H43, """",", ", """",I43, """",", ", """",J43, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "भागो रे जग से अब भागो", "Bhago Re Jag Se Ab Bhago", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "30", "चितावनी", "Admonition", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Bhago Re Jag Se Ab Bhago.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bhago Re Jag Se Ab Bhago.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18741,7 +18743,7 @@
         <v>678</v>
       </c>
       <c r="K44" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A44, """",", ", """", B44, """",", ", """",C44, """",", ", """",D44, """",", ", """",E44, """",", ", """",F44, """",", ", """",G44, """",", ", """",H44, """",", ", """",I44, """",", ", """",J44, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "चेतो रे घर घाट सम्हारो", "Cheto Re Ghar Ghat Samharo", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "31", "चितावनी", "Admonition", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Cheto Re Ghar Ghat Samharo.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Cheto Re Ghar Ghat Samharo.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18777,7 +18779,7 @@
         <v>679</v>
       </c>
       <c r="K45" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A45, """",", ", """", B45, """",", ", """",C45, """",", ", """",D45, """",", ", """",E45, """",", ", """",F45, """",", ", """",G45, """",", ", """",H45, """",", ", """",I45, """",", ", """",J45, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "जागो रे यहाँ कब लग सोना", "Jago Re Yehan Kab Lag Sona", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "32", "चितावनी", "Admonition", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Jago Re Yehan Kab Lag Sona.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jago Re Yehan Kab Lag Sona.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18813,7 +18815,7 @@
         <v>680</v>
       </c>
       <c r="K46" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A46, """",", ", """", B46, """",", ", """",C46, """",", ", """",D46, """",", ", """",E46, """",", ", """",F46, """",", ", """",G46, """",", ", """",H46, """",", ", """",I46, """",", ", """",J46, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "प्रेम दात गुरु दीजिये मेरे समरथ दाता हो", "Prem Dat Guru Dijiye Mere Samrath Data Ho", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "60", "फ़र्याद एवं पुकार, नियमावली", "Invocation, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Prem Dat Guru Dijiye Mere Samrath Data Ho.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Prem Dat Guru Dijiye Mere Samrath Data Ho.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18849,7 +18851,7 @@
         <v>681</v>
       </c>
       <c r="K47" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A47, """",", ", """", B47, """",", ", """",C47, """",", ", """",D47, """",", ", """",E47, """",", ", """",F47, """",", ", """",G47, """",", ", """",H47, """",", ", """",I47, """",", ", """",J47, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "हे मेरे समरथ साईं निज रूप दिखाओ", "He Mere Samarath Saeen Nij Roop Dikhao", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "80", "प्रेम एवं विरह", "Love and Yearning", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/He Mere Samarath Saeen Nij Roop Dikhao.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/He Mere Samarath Saeen Nij Roop Dikhao.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18885,7 +18887,7 @@
         <v>682</v>
       </c>
       <c r="K48" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A48, """",", ", """", B48, """",", ", """",C48, """",", ", """",D48, """",", ", """",E48, """",", ", """",F48, """",", ", """",G48, """",", ", """",H48, """",", ", """",I48, """",", ", """",J48, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "जो मेरे प्रीतम से प्रीत करे", "Jo Mere Preetam Se Preet Kare", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "82", "फ़र्याद एवं पुकार", "Invocation", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Jo Mere Preetam Se Preet Kare.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jo Mere Preetam Se Preet Kare.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18921,7 +18923,7 @@
         <v>683</v>
       </c>
       <c r="K49" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A49, """",", ", """", B49, """",", ", """",C49, """",", ", """",D49, """",", ", """",E49, """",", ", """",F49, """",", ", """",G49, """",", ", """",H49, """",", ", """",I49, """",", ", """",J49, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "जगत जीव सब होली पूजें", "Jagat Jeev Sab Holi Poojen", "प्रेम बानी, भाग 4", "Prem Bani, Part - 4", "40", "84", "होली सत्संग", "Holi Satang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Jagat Jeev Sab Holi Poojen.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Jagat Jeev Sab Holi Poojen.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18954,7 +18956,7 @@
         <v>684</v>
       </c>
       <c r="K50" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A50, """",", ", """", B50, """",", ", """",C50, """",", ", """",D50, """",", ", """",E50, """",", ", """",F50, """",", ", """",G50, """",", ", """",H50, """",", ", """",I50, """",", ", """",J50, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "राधास्वामी नाम जो गावे सो ही तरे", "Radhasoami Naam Jo Gave So Hi Tare", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "3", "", "मंगलाचरण एवं बिनती", "Manglacharan and Prayer", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Radhasoami Naam Jo Gave So Hi Tare.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Radhasoami Naam Jo Gave So Hi Tare.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -18990,7 +18992,7 @@
         <v>685</v>
       </c>
       <c r="K51" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A51, """",", ", """", B51, """",", ", """",C51, """",", ", """",D51, """",", ", """",E51, """",", ", """",F51, """",", ", """",G51, """",", ", """",H51, """",", ", """",I51, """",", ", """",J51, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "आज बधावा राधास्वामी गाऊँ", "Aaj Badhawa Radhasoami Gaoon", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "4", "2", "बधावा एवं शुकराना", "Thanksgiving", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Badhawa Radhasoami Gaoon.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Badhawa Radhasoami Gaoon.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19026,7 +19028,7 @@
         <v>686</v>
       </c>
       <c r="K52" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A52, """",", ", """", B52, """",", ", """",C52, """",", ", """",D52, """",", ", """",E52, """",", ", """",F52, """",", ", """",G52, """",", ", """",H52, """",", ", """",I52, """",", ", """",J52, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "आज मेरे धूम भई है भारी", "Aaj Mere Dhoom Bhai Hai Bhari", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "4", "3", "शादी व अन्य खुशी के मौके", "Marriage and Other Happy Occasions", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Mere Dhoom Bhai Hai Bhari.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Mere Dhoom Bhai Hai Bhari.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19062,7 +19064,7 @@
         <v>687</v>
       </c>
       <c r="K53" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A53, """",", ", """", B53, """",", ", """",C53, """",", ", """",D53, """",", ", """",E53, """",", ", """",F53, """",", ", """",G53, """",", ", """",H53, """",", ", """",I53, """",", ", """",J53, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "आज साज कर आरत लाई", "Aaj Saj Kar Aarat Laee", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "6", "4", "भंडारा महाराज साहब, सत्संग आसाढ़ बदी पड़िवा", "Bhandara of Maharaj Saheb, Satsang on Asadh Badi Padiwa", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Saj Kar Aarat Laee.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Saj Kar Aarat Laee.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19098,7 +19100,7 @@
         <v>688</v>
       </c>
       <c r="K54" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A54, """",", ", """", B54, """",", ", """",C54, """",", ", """",D54, """",", ", """",E54, """",", ", """",F54, """",", ", """",G54, """",", ", """",H54, """",", ", """",I54, """",", ", """",J54, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "आनँद मंगल आज साज सब आरत लाई", "Anand Mangal Aaj Saj Sab Aarat Laee", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "6", "6", "भंडारा बाबूजी महाराज", "Bhandara of Babuji Maharaj", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Anand Mangal Aaj Saj Sab Aarat Laee.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Anand Mangal Aaj Saj Sab Aarat Laee.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19134,7 +19136,7 @@
         <v>689</v>
       </c>
       <c r="K55" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A55, """",", ", """", B55, """",", ", """",C55, """",", ", """",D55, """",", ", """",E55, """",", ", """",F55, """",", ", """",G55, """",", ", """",H55, """",", ", """",I55, """",", ", """",J55, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "करूँ आरती राधास्वामी तन मन सुरत लगाय", "Karoon Arti Radhasoami Tan Man Surat Lagay", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "6", "7", "भंडारा महाराज साहब, भंडारा बाबूजी महाराज, आरतियाँ राधाजी महाराज, सत्संग आसाढ़ बदी पड़िवा", "Bhandara of Maharaj Saheb, Bhandara of Babuji Maharaj, Arti of Radhaji Maharaj ", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Karoon Arti Radhasoami Tan Man Surat Lagay.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Karoon Arti Radhasoami Tan Man Surat Lagay.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19170,7 +19172,7 @@
         <v>690</v>
       </c>
       <c r="K56" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A56, """",", ", """", B56, """",", ", """",C56, """",", ", """",D56, """",", ", """",E56, """",", ", """",F56, """",", ", """",G56, """",", ", """",H56, """",", ", """",I56, """",", ", """",J56, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "आरत करूँ आज सतगुरु की", "Aarat Karoon Aaj Satguru Ki", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "6", "15", "भंडारा बुआजी महाराज", "Bhandara of Buaji Maharaj", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aarat Karoon Aaj Satguru Ki.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aarat Karoon Aaj Satguru Ki.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19206,7 +19208,7 @@
         <v>691</v>
       </c>
       <c r="K57" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A57, """",", ", """", B57, """",", ", """",C57, """",", ", """",D57, """",", ", """",E57, """",", ", """",F57, """",", ", """",G57, """",", ", """",H57, """",", ", """",I57, """",", ", """",J57, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "करूँ बीनती दोउ कर जोरी", "Karoon Binti Dou Kar Jori", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "7", "1", "मंगलाचरण एवं बिनती", "Manglacharan and Prayer", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Karoon Binti Dou Kar Jori.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Karoon Binti Dou Kar Jori.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19242,7 +19244,7 @@
         <v>692</v>
       </c>
       <c r="K58" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A58, """",", ", """", B58, """",", ", """",C58, """",", ", """",D58, """",", ", """",E58, """",", ", """",F58, """",", ", """",G58, """",", ", """",H58, """",", ", """",I58, """",", ", """",J58, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "आज मेरे आनँद होत अपार", "Aaj Mere Anand Hot Apar", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "8", "4", "भंडारा हुज़ूर महाराज", "Bhandara of Huzur Maharaj", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Mere Anand Hot Apar.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Mere Anand Hot Apar.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19278,7 +19280,7 @@
         <v>693</v>
       </c>
       <c r="K59" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A59, """",", ", """", B59, """",", ", """",C59, """",", ", """",D59, """",", ", """",E59, """",", ", """",F59, """",", ", """",G59, """",", ", """",H59, """",", ", """",I59, """",", ", """",J59, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "गुरु की कर हर दम पूजा", "Guru Ki Kar Har Dam Pooja", "सार बचन छंद बंद, भाग 1", "Sar Bachan Poetry, Part-1", "18", "2", "सत्संग गुरु पूर्णिमा", "Guru Purnima Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Guru Ki Kar Har Dam Pooja.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Ki Kar Har Dam Pooja.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19314,7 +19316,7 @@
         <v>694</v>
       </c>
       <c r="K60" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A60, """",", ", """", B60, """",", ", """",C60, """",", ", """",D60, """",", ", """",E60, """",", ", """",F60, """",", ", """",G60, """",", ", """",H60, """",", ", """",I60, """",", ", """",J60, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "दर्द दुखी मैं बिरहिन भारी", "Dard Dukhi Main Birahin Bhari", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "27", "2", "प्रेम एवं विरह", "Satsang on Asadh Badi Padiwa, Love and Yearning ", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Dard Dukhi Main Birahin Bhari.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Dard Dukhi Main Birahin Bhari.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19350,7 +19352,7 @@
         <v>695</v>
       </c>
       <c r="K61" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A61, """",", ", """", B61, """",", ", """",C61, """",", ", """",D61, """",", ", """",E61, """",", ", """",F61, """",", ", """",G61, """",", ", """",H61, """",", ", """",I61, """",", ", """",J61, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "पिया बिन कैसे जिऊँ मैं प्यारी", "Piya Bin Kaise Jioon Main Pyari", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "27", "4", "प्रेम एवं विरह", "Satsang on Asadh Badi Padiwa, Love and Yearning", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Piya Bin Kaise Jioon Main Pyari.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Piya Bin Kaise Jioon Main Pyari.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19386,7 +19388,7 @@
         <v>696</v>
       </c>
       <c r="K62" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A62, """",", ", """", B62, """",", ", """",C62, """",", ", """",D62, """",", ", """",E62, """",", ", """",F62, """",", ", """",G62, """",", ", """",H62, """",", ", """",I62, """",", ", """",J62, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "चुनर मेरी मैली भई", "Chunar Meri Maili Bhayee", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "27", "6", "प्रेम एवं विरह", "Love and Yearning", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Chunar Meri Maili Bhayee.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Chunar Meri Maili Bhayee.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19422,7 +19424,7 @@
         <v>697</v>
       </c>
       <c r="K63" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A63, """",", ", """", B63, """",", ", """",C63, """",", ", """",D63, """",", ", """",E63, """",", ", """",F63, """",", ", """",G63, """",", ", """",H63, """",", ", """",I63, """",", ", """",J63, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "आज घड़ी अति पावन भावन", "Aaj Ghadi Ati Pawan Bhavan", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "28", "4", "गृह प्रवेश", "House warming", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Ghadi Ati Pawan Bhavan.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Ghadi Ati Pawan Bhavan.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19458,7 +19460,7 @@
         <v>698</v>
       </c>
       <c r="K64" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A64, """",", ", """", B64, """",", ", """",C64, """",", ", """",D64, """",", ", """",E64, """",", ", """",F64, """",", ", """",G64, """",", ", """",H64, """",", ", """",I64, """",", ", """",J64, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "गुरु चरन गिरह मेरे आये", "Guru Charan Girah Mere Aaye", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "28", "5", "गृह प्रवेश", "House warming", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Guru Charan Girah Mere Aaye.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Charan Girah Mere Aaye.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19494,7 +19496,7 @@
         <v>699</v>
       </c>
       <c r="K65" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A65, """",", ", """", B65, """",", ", """",C65, """",", ", """",D65, """",", ", """",E65, """",", ", """",F65, """",", ", """",G65, """",", ", """",H65, """",", ", """",I65, """",", ", """",J65, """"," ]")</f>
+        <f t="shared" si="1"/>
         <v>[ "कौन करे आरत सतगुरु की", "Kaun Kare Aarat Satguru Ki", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "28", "6", "सत्संग गुरु पूर्णिमा", "Guru Purnima Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Kaun Kare Aarat Satguru Ki.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Kaun Kare Aarat Satguru Ki.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19530,7 +19532,7 @@
         <v>700</v>
       </c>
       <c r="K66" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A66, """",", ", """", B66, """",", ", """",C66, """",", ", """",D66, """",", ", """",E66, """",", ", """",F66, """",", ", """",G66, """",", ", """",H66, """",", ", """",I66, """",", ", """",J66, """"," ]")</f>
+        <f t="shared" ref="K66:K97" si="2">_xlfn.CONCAT("[ ", """", A66, """",", ", """", B66, """",", ", """",C66, """",", ", """",D66, """",", ", """",E66, """",", ", """",F66, """",", ", """",G66, """",", ", """",H66, """",", ", """",I66, """",", ", """",J66, """"," ]")</f>
         <v>[ "गुरु मैं गुनहगार अति भारी", "Guru Main Gunahagar Ati Bhari", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "29", "3", "रात को सोने से पहले, नियमावली", "Before retiring to bed in evening, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Guru Main Gunahagar Ati Bhari.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Guru Main Gunahagar Ati Bhari.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19563,7 +19565,7 @@
         <v>701</v>
       </c>
       <c r="K67" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A67, """",", ", """", B67, """",", ", """",C67, """",", ", """",D67, """",", ", """",E67, """",", ", """",F67, """",", ", """",G67, """",", ", """",H67, """",", ", """",I67, """",", ", """",J67, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "आरत गाऊँ पूरे गुरु की", "Aarat Gaoon Poore Guru Ki", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "30", "2", "", "Arti Shabd", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aarat Gaoon Poore Guru Ki.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aarat Gaoon Poore Guru Ki.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19596,7 +19598,7 @@
         <v>702</v>
       </c>
       <c r="K68" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A68, """",", ", """", B68, """",", ", """",C68, """",", ", """",D68, """",", ", """",E68, """",", ", """",F68, """",", ", """",G68, """",", ", """",H68, """",", ", """",I68, """",", ", """",J68, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "राधास्वामी राधास्वामी राधास्वामी गाऊँ", "Radhasoami Radhasoami Radhasoami Gaoon", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "30", "3", "", "Ari Shabd", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Radhasoami Radhasoami Radhasoami Gaoon.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Radhasoami Radhasoami Radhasoami Gaoon.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19629,7 +19631,7 @@
         <v>703</v>
       </c>
       <c r="K69" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A69, """",", ", """", B69, """",", ", """",C69, """",", ", """",D69, """",", ", """",E69, """",", ", """",F69, """",", ", """",G69, """",", ", """",H69, """",", ", """",I69, """",", ", """",J69, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "गाऊँ आरती लेकर थाली", "Gaoon Arti Lekar Thali", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "30", "5", "", "Arti Shabd", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Gaoon Arti Lekar Thali.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Gaoon Arti Lekar Thali.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19662,7 +19664,7 @@
         <v>704</v>
       </c>
       <c r="K70" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A70, """",", ", """", B70, """",", ", """",C70, """",", ", """",D70, """",", ", """",E70, """",", ", """",F70, """",", ", """",G70, """",", ", """",H70, """",", ", """",I70, """",", ", """",J70, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "आज आरती करूँ सुहावन", "Aaj Arti Karoon Suhawan", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "30", "18", "", "Arti Shabd", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Arti Karoon Suhawan.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Arti Karoon Suhawan.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19698,7 +19700,7 @@
         <v>705</v>
       </c>
       <c r="K71" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A71, """",", ", """", B71, """",", ", """",C71, """",", ", """",D71, """",", ", """",E71, """",", ", """",F71, """",", ", """",G71, """",", ", """",H71, """",", ", """",I71, """",", ", """",J71, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "अब मन आतुर दरस पुकारे", "Ab Man Aatur Daras Pukare", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "33", "1", "फ़र्याद एवं पुकार", "Invocation", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Ab Man Aatur Daras Pukare.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ab Man Aatur Daras Pukare.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19731,7 +19733,7 @@
         <v>706</v>
       </c>
       <c r="K72" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A72, """",", ", """", B72, """",", ", """",C72, """",", ", """",D72, """",", ", """",E72, """",", ", """",F72, """",", ", """",G72, """",", ", """",H72, """",", ", """",I72, """",", ", """",J72, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "अब मैं कौन कुमति उरझानी", "Ab Main Kaun Kumati Urjhani", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "33", "2", "", "invocation", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Ab Main Kaun Kumati Urjhani.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ab Main Kaun Kumati Urjhani.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19767,7 +19769,7 @@
         <v>707</v>
       </c>
       <c r="K73" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A73, """",", ", """", B73, """",", ", """",C73, """",", ", """",D73, """",", ", """",E73, """",", ", """",F73, """",", ", """",G73, """",", ", """",H73, """",", ", """",I73, """",", ", """",J73, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "करत हूँ पुकार आज सुनिये गुहार", "Karat Hoon Pukar Aaj Suniye Guhar", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "33", "3", "सुबह उठने के बाद, नियमावली", "After waking up in morning, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Karat Hoon Pukar Aaj Suniye Guhar.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Karat Hoon Pukar Aaj Suniye Guhar.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19803,7 +19805,7 @@
         <v>708</v>
       </c>
       <c r="K74" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A74, """",", ", """", B74, """",", ", """",C74, """",", ", """",D74, """",", ", """",E74, """",", ", """",F74, """",", ", """",G74, """",", ", """",H74, """",", ", """",I74, """",", ", """",J74, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "लगाओ मेरी नइया सतगुरु पार", "Lagao Meri Naiya Satguru Par", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "33", "20", "अंतिम समय एवं मृत्यु", "Illness and End Time or Death ", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Lagao Meri Naiya Satguru Par.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Lagao Meri Naiya Satguru Par.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19836,7 +19838,7 @@
         <v>709</v>
       </c>
       <c r="K75" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A75, """",", ", """", B75, """",", ", """",C75, """",", ", """",D75, """",", ", """",E75, """",", ", """",F75, """",", ", """",G75, """",", ", """",H75, """",", ", """",I75, """",", ", """",J75, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "धीरज धरना मत घबराना", "Dhiraj Dharana Mat Ghabrana", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "33", "", "भंडारा हुज़ूर महाराज, नियमावली", "Bhandara of Huzur Maharaj, Niyamawali", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Dhiraj Dharana Mat Ghabrana.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Dhiraj Dharana Mat Ghabrana.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19872,7 +19874,7 @@
         <v>710</v>
       </c>
       <c r="K76" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A76, """",", ", """", B76, """",", ", """",C76, """",", ", """",D76, """",", ", """",E76, """",", ", """",F76, """",", ", """",G76, """",", ", """",H76, """",", ", """",I76, """",", ", """",J76, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "आज काज मेरे कीन्हे पूरे", "Aaj Kaj Mere Kinhe Poore", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "34", "2", "प्रार्थना दया एवं मेहर के लिये", "Prayer for Daya and Mehar", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aaj Kaj Mere Kinhe Poore.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aaj Kaj Mere Kinhe Poore.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19908,7 +19910,7 @@
         <v>711</v>
       </c>
       <c r="K77" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A77, """",", ", """", B77, """",", ", """",C77, """",", ", """",D77, """",", ", """",E77, """",", ", """",F77, """",", ", """",G77, """",", ", """",H77, """",", ", """",I77, """",", ", """",J77, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "आओ री सिमट हे सखियो", "Aao Ri Simat He Sakhiyo", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "34", "13", "प्रार्थना दया एवं मेहर के लिये", "Prayer for Daya and Mehar", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aao Ri Simat He Sakhiyo.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aao Ri Simat He Sakhiyo.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19944,7 +19946,7 @@
         <v>712</v>
       </c>
       <c r="K78" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A78, """",", ", """", B78, """",", ", """",C78, """",", ", """",D78, """",", ", """",E78, """",", ", """",F78, """",", ", """",G78, """",", ", """",H78, """",", ", """",I78, """",", ", """",J78, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "घट में खेलूँ अब बसन्त", "Ghat Mein Kheloon Ab Basant", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "39", "2", "बसंत पंचमी सत्संग", "Basant Panchmi Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Ghat Mein Kheloon Ab Basant.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ghat Mein Kheloon Ab Basant.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -19980,7 +19982,7 @@
         <v>713</v>
       </c>
       <c r="K79" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A79, """",", ", """", B79, """",", ", """",C79, """",", ", """",D79, """",", ", """",E79, """",", ", """",F79, """",", ", """",G79, """",", ", """",H79, """",", ", """",I79, """",", ", """",J79, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "देखन चली बसंत अगम घर", "Dekhan Chali Basant Agam Ghar", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "39", "4", "बसंत पंचमी सत्संग", "Basant Panchmi Satsang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Dekhan Chali Basant Agam Ghar.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Dekhan Chali Basant Agam Ghar.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -20016,7 +20018,7 @@
         <v>714</v>
       </c>
       <c r="K80" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A80, """",", ", """", B80, """",", ", """",C80, """",", ", """",D80, """",", ", """",E80, """",", ", """",F80, """",", ", """",G80, """",", ", """",H80, """",", ", """",I80, """",", ", """",J80, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "अब खेलत राधास्वामी सँग होरी", "Ab Khelat Radhasoami Sang Hori", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "39", "5", "होली सत्संग", "Holi Satang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Ab Khelat Radhasoami Sang Hori.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ab Khelat Radhasoami Sang Hori.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -20052,7 +20054,7 @@
         <v>715</v>
       </c>
       <c r="K81" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A81, """",", ", """", B81, """",", ", """",C81, """",", ", """",D81, """",", ", """",E81, """",", ", """",F81, """",", ", """",G81, """",", ", """",H81, """",", ", """",I81, """",", ", """",J81, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "आओ री सखी जुड़ होली गावें", "Aao Ri Sakhi Jud Holi Gaven", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "39", "12", "होली सत्संग", "Holi Satang", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Aao Ri Sakhi Jud Holi Gaven.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Aao Ri Sakhi Jud Holi Gaven.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -20088,7 +20090,7 @@
         <v>716</v>
       </c>
       <c r="K82" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A82, """",", ", """", B82, """",", ", """",C82, """",", ", """",D82, """",", ", """",E82, """",", ", """",F82, """",", ", """",G82, """",", ", """",H82, """",", ", """",I82, """",", ", """",J82, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "अजब यह बँगला लिया सजाय", "Ajab Yeh Bangla Liya Sajay", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "40", "5", "गृह प्रवेश", "House warming", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Ajab Yeh Bangla Liya Sajay.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Ajab Yeh Bangla Liya Sajay.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -20124,7 +20126,7 @@
         <v>717</v>
       </c>
       <c r="K83" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A83, """",", ", """", B83, """",", ", """",C83, """",", ", """",D83, """",", ", """",E83, """",", ", """",F83, """",", ", """",G83, """",", ", """",H83, """",", ", """",I83, """",", ", """",J83, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "चौका बरतन किया अचंभी", "Chauka Bartan Kiya Achambhi", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "42", "2", "सेवा बानी", "Hyms of Sewa", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Chauka Bartan Kiya Achambhi.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Chauka Bartan Kiya Achambhi.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>
@@ -20160,7 +20162,7 @@
         <v>718</v>
       </c>
       <c r="K84" t="str">
-        <f>_xlfn.CONCAT("[ ", """", A84, """",", ", """", B84, """",", ", """",C84, """",", ", """",D84, """",", ", """",E84, """",", ", """",F84, """",", ", """",G84, """",", ", """",H84, """",", ", """",I84, """",", ", """",J84, """"," ]")</f>
+        <f t="shared" si="2"/>
         <v>[ "भोग धरे राधास्वामी आगे", "Bhog Dhare Radhasoami Aage", "सार बचन छंद बंद, भाग 2", "Sar Bachan Poetry, Part-2", "42", "4", "भोग", "Bhog", "&lt;a href='http://radhasoamifaith.org/Audio/Shabd/Bhog Dhare Radhasoami Aage.mp3'&gt;Audio&lt;/a&gt;", "&lt;a href='http://radhasoamifaith.org/Video/Poetry/Bhog Dhare Radhasoami Aage.mp4'&gt;Video&lt;/a&gt;" ]</v>
       </c>
     </row>

</xml_diff>